<commit_message>
#docs updated mkdocs links
</commit_message>
<xml_diff>
--- a/docs/datasets/tweet_dataset.xlsx
+++ b/docs/datasets/tweet_dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="182">
   <si>
     <t>Tweet</t>
   </si>
@@ -37,648 +37,610 @@
     <t>Hashtags</t>
   </si>
   <si>
-    <t>I believe most of the #TSLA community &amp;amp; members of @SpaceX see the writing on the wall…but unfortunately &amp;amp; honestly quite understandably the message can be misconstrued a little bit as it passes through the grape-vine 🍇</t>
-  </si>
-  <si>
-    <t>Shoutout to my girl @SpeakerPelosi!
-You are rocking that #TSLA trade 💵</t>
-  </si>
-  <si>
-    <t>Our longer term swing trading portfolio now consists of a buy signal for #TSLA and sell signals for #ES. #NASDAQ, #DXY, #Gold, #Silver, #CrudeOil and #Soybeans</t>
-  </si>
-  <si>
-    <t>TESLA has made a deal with nickel miner! Essential mineral for batteries 🔋 $VALE, trading at $20, it looks very promising for go up👆🏼Im adding calls here for May 2022, 21 calls at 0.93.
-#spy #tsla #minerals #vale #copper #uraniumsqueeze $TSLA $VALE</t>
-  </si>
-  <si>
-    <t>$tsla -  Did anyone else see this?? This is huge IMO!
-#tesla #tsla #teslastock 
-Tesla Dodges Nickel Crisis With Secret Deal to Get Supplies https://t.co/shqOOgEXZX via @YahooFinanceCA</t>
-  </si>
-  <si>
-    <t>Tesla has to split at this point it’s so high #TSLA #Doge</t>
-  </si>
-  <si>
-    <t>@squawksquare Same thinking and look like it though #tsla #pltr</t>
-  </si>
-  <si>
-    <t>#tsla $Tsla sold 1150c at 9.1. Felt too risky. Exited early</t>
-  </si>
-  <si>
-    <t>@patienttrading I love this $2222.22 …..#tsla</t>
-  </si>
-  <si>
-    <t>It will end with them losing all their money. #TSLA $TSLA https://t.co/UI8Iz622tO</t>
-  </si>
-  <si>
-    <t>$TSLA is booming in impressions the last 4hrs - Price is back to its spot over 1100k - Seeing high volume here as well - Let's end today green! #TSLA 
-https://t.co/nNt764nQuW https://t.co/1xjzxO6mH1</t>
-  </si>
-  <si>
-    <t>Lookin like a hot tamale 🥵
-#AMC #GME #TLRY #TSLA</t>
-  </si>
-  <si>
-    <t>#TSLA $TSLA 1150c entered at 8.45 Friday expiration</t>
-  </si>
-  <si>
-    <t>$TSLA   Subscribe now: https://t.co/bPB4JlRYZs
-#TSLA #InvexGlobal #OptionsTrading #Options #NASDAQ #NYSE #trading #stocks #daytrading #market #investors #USA https://t.co/4jZemrwSiD</t>
-  </si>
-  <si>
-    <t>Tesla is handy as a smart phone. Power of engineering @elonmusk .
-#tsla #tesla</t>
-  </si>
-  <si>
-    <t>BIDEN POISED TO USE COLD-WAR POWERS TO DEVELOP BATTERY METALS #TSLA #TESLA @elonmusk</t>
-  </si>
-  <si>
-    <t>@talesftf @StanphylCap @munster_gene Lending the FSD platform planned by #TSLA is definitely not done by them but #NVDA  https://t.co/7JrWgCqmUY 
-https://t.co/RAHmGDtVyz</t>
-  </si>
-  <si>
-    <t>@LukasMertens10 Innovation drives product demand. #ElonMusk #TSLA</t>
-  </si>
-  <si>
-    <t>“People don’t realize how far ahead @Tesla is when it comes to securing the supply chain for raw materials and an integrated approach to #battery materials,” said Todd Malan, a spokesman for @TalonMetals
-#Tesla @elonmusk #TSLA #Investor #EVs
-https://t.co/zOARD4WyVH via @Yahoo</t>
-  </si>
-  <si>
-    <t>Just got an offer for the installation of a #Tesla powerwall 2 as an addition to my #solar roof 😁 - am hyped to do even more good for the planet! #renewableenergy #renewables #tsla https://t.co/5qHjPG0ysf</t>
-  </si>
-  <si>
-    <t>@squawksquare Let’s go #tsla</t>
-  </si>
-  <si>
-    <t>#nio is up 3% and #expv more than 5% - not a bad way to start a day on Wallstreet $NIO $EXPV #tsla https://t.co/3gm1ORt1UW</t>
-  </si>
-  <si>
-    <t>#spy $SPY #SPX $SPX $QQQ #QQQ #ES_F $ES_F #NQ_F $NQ_F $VIX #VIX $AAPL #AAPL $MSFT #MSFT $GOOGL #GOOGL $AMZN #AMZN $FB #FB $TLT #TLT $MOVE $ARKK #ARKK $TSLA #TSLA Out of ARKK lottos at breakeven. Saving bullets for next time. Will buy some weekly puts when TSLA gets to resistance https://t.co/gfufQMTswa https://t.co/vEkl9qzvNC</t>
-  </si>
-  <si>
-    <t>#TSLA inked a multiyear supply deal with mining giant #VALE long before the Russia-Ukraine war as part of the electric vehicle maker's global hunt for nickel.
-Over the last year, #TSLA has also secured nickel supply deals with #BHP and operators of a mine in New Caledonia.</t>
-  </si>
-  <si>
-    <t>Might retest $1055 area. Let’s break that down trend.
-#tsla $tsla https://t.co/NJEjWU4ft6</t>
-  </si>
-  <si>
-    <t>Stock Market Timing 20220330 #Natural_Gas #Crude_Oil #Gold #Silver #TSX #SPY #QQQ #TSLA #SHOP.TO #Trading https://t.co/u3vGhGDIbZ</t>
-  </si>
-  <si>
-    <t>Tesla Dodges Nickel Crisis With Secret Deal to Get Supplies https://t.co/HzkHqgHtQQ 
-#CanadaNickel 
-#SudburyTwoPointO
-#NetZeroNickel 
-#TM  #Nickel  $CNIKF
-$NOB.V $SHL.V $CNC.V  #EV #BatteryMetals   #Reddit #TSLA #ESG #Mining #ElonMusk 
-#Glencore #BHP #Vale #Timmins #Canada https://t.co/r1u1aVJIcD</t>
-  </si>
-  <si>
-    <t>3 Clean Energy Stocks to Buy for a Green Future $TSLA #TSLA #cleanenergy #energy #fossilfuels https://t.co/RYEEVBKBii</t>
-  </si>
-  <si>
-    <t>More of the same AH from $TSLA #TSLA https://t.co/UYL1MXKWhi</t>
-  </si>
-  <si>
-    <t>⭐️Option Trade Ideas 3/30⭐️
-$AAL
-CALLS OVER  $18.30
-PUTS BELOW $17.85
-$FUBO
-CALLS OVER  $7.80
-PUTS BELOW $7.50
-$FB 
-CALLS OVER  $229.20
-PUTS BELOW $226.90
-$DOCU
-CALLS OVER  $111.75 (possible Swing)
-ON WATCH: $RBLX, $TSLA, $SPY⭐️
-#OptionsTrading #TSLA 🤘</t>
-  </si>
-  <si>
-    <t>Stocks Picks of the Day 
-#BNTX -up 
-#CHWY -down 
-#LULU -up
-#TSLA -down 
-Opening red market #fypシ #tiktok #viral #stockmarket #stocks #tranding #fanpage #BTCUSD #DowJones #Futures #forextrading #NASDAQ #GameStop #AMCSTOCK https://t.co/qKockhrKNc</t>
-  </si>
-  <si>
-    <t>#TSLA - #CEDEAR - update
-👇
-https://t.co/atccZX4Hof
-#EEUU #tecnología #research https://t.co/qoCcWFUkJ3</t>
-  </si>
-  <si>
-    <t>3/30 Daily Watchlist #TSLA #AMC #CRWD #TAN #W @unusual_whales @Stocktwits #StocksToWatch #DayTrading #OptionsTrading #Options https://t.co/VsEZYlqmqD</t>
-  </si>
-  <si>
-    <t>Watching #TSLA https://t.co/bpkt3zlriv</t>
-  </si>
-  <si>
-    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/X3mJvhSzdb</t>
-  </si>
-  <si>
-    <t>#Tesla #tsla manufacturing prowess, stock #split plans indicate ‘massive position of strength:’ #Wedbush
-https://t.co/ozuPkOSvC1</t>
-  </si>
-  <si>
-    <t>“I think #TSLA is one of the least efficient manufacturers of cars.”        - 🤡 https://t.co/sROzi8CaGy</t>
-  </si>
-  <si>
-    <t>With the #Tesla #Model2, electric car ownership looks set to become more affordable. But what else can be expected from this upcoming #electricvehicle? 😎
-#tsla #elon #elonmusk #electriccar #cars #carnews #driving 
-https://t.co/a57DasYEaG</t>
-  </si>
-  <si>
-    <t>$TSLA was the 4th most mentioned on wallstreetbets over the last 7 days_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #trading https://t.co/H43JzzM3Ad</t>
-  </si>
-  <si>
-    <t>Q1 Production &amp;amp; Delivery Estimate - I am once again a bit of an outlier, but I have reasonable confidence in the conclusion. I'm working on the companion video explaining it for today. 328,187
-#tsla #tesla #Q12022 @bradsferguson @elonmusk https://t.co/oQFYtirXTK</t>
-  </si>
-  <si>
-    <t>Thoughts on $TSLA #TSLA! See zeyankhan1318's idea on TradingView below. https://t.co/nspRUd6puv</t>
-  </si>
-  <si>
-    <t>$TSLA Stock Split!!!
- Here's what you need to know:
-https://t.co/amvs2gVhEN
-#tsla #teslastock #StockMarket #StockSplit #fintwit #FinTwitt</t>
-  </si>
-  <si>
-    <t>#TESLA #TSLA CHART REQUEST
-If trading leverage, consider taking some profit at current level. Likely to pullback to fill the parabola (lower range consolidation). If parabola remains intact, this could go to $1979 in a very short time. Risk manage at all times. All the best https://t.co/EtLgLsPj7z</t>
-  </si>
-  <si>
-    <t>Wednesday,  March 30, 2022
-Daily Market Correction : 
-🌙  Waning 5% in ♓️ 🍅 
-🐻‍❄️: 0654 - 0900 EST 
-🐃: 1002 - 1208 EST 
-🐻‍❄️: 1413 - 1619 EST
-🐃: 1722 - 1927 EST
-🐻‍❄️: 2121 - 2316 EST 
-$SPY #sp500 #Bitcoin $AAPL $NVDA $MSFT #TSLA #NASDAQ 
-(not financial advice)</t>
-  </si>
-  <si>
-    <t>@alex_avoigt But, but Gordon said the opening of Giga Berlin was a stock pump.  Berlin won’t deliver any cars anytime soon #TSLAQ #TSLA</t>
-  </si>
-  <si>
-    <t>#BTC #TSLA 
-Let's start to prepare NYO
-- $DXY : BreakDown Trend
-- $USOIL : Key-Horizontal level
-- $VIX : Dump. but support level
-- $GOLD : Range Low
-US stock 
-- $QQQ : HOLD around Range High
-- $AMD : No problem(imo)
-Crypto
-- $BTC : HOLD near RH https://t.co/bJaL3TI5YB</t>
-  </si>
-  <si>
-    <t>I want to buy #tsla</t>
-  </si>
-  <si>
-    <t>Is #TSLA a buy, hold or sell in its current value? #teslastock</t>
-  </si>
-  <si>
-    <t>@hikingskiing they direct listed, so institutional wallstreet does not like them.  i hold them long term, and software is high margin.  got #tsla back in 2010, and people were saying the same thing for many years.  same for #btc back in 2015.  hmm 🤔😂😂. HODL'ong &amp;amp; HODL'hard 👊👊</t>
-  </si>
-  <si>
-    <t>Have a look #Elonmusk #tsla #audi #volkswagen #porsche #mercedes #panasonic #varta #bmw #recycling #recycle #electricvehicle #batteries https://t.co/JifoClSnEj</t>
-  </si>
-  <si>
-    <t>30-03-2022 15:42</t>
-  </si>
-  <si>
-    <t>30-03-2022 15:41</t>
-  </si>
-  <si>
-    <t>30-03-2022 15:23</t>
-  </si>
-  <si>
-    <t>30-03-2022 15:03</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:57</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:53</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:42</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:38</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:32</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:30</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:26</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:24</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:17</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:13</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:11</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:07</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:06</t>
-  </si>
-  <si>
-    <t>30-03-2022 14:02</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:57</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:48</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:38</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:26</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:25</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:21</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:11</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:08</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:04</t>
-  </si>
-  <si>
-    <t>30-03-2022 13:01</t>
-  </si>
-  <si>
-    <t>30-03-2022 12:49</t>
-  </si>
-  <si>
-    <t>30-03-2022 12:41</t>
-  </si>
-  <si>
-    <t>30-03-2022 12:35</t>
-  </si>
-  <si>
-    <t>30-03-2022 12:23</t>
-  </si>
-  <si>
-    <t>30-03-2022 12:19</t>
-  </si>
-  <si>
-    <t>30-03-2022 11:46</t>
-  </si>
-  <si>
-    <t>30-03-2022 11:25</t>
-  </si>
-  <si>
-    <t>30-03-2022 11:24</t>
-  </si>
-  <si>
-    <t>30-03-2022 10:33</t>
-  </si>
-  <si>
-    <t>30-03-2022 10:20</t>
-  </si>
-  <si>
-    <t>30-03-2022 10:15</t>
-  </si>
-  <si>
-    <t>30-03-2022 10:11</t>
-  </si>
-  <si>
-    <t>30-03-2022 09:34</t>
-  </si>
-  <si>
-    <t>30-03-2022 09:32</t>
-  </si>
-  <si>
-    <t>30-03-2022 09:28</t>
-  </si>
-  <si>
-    <t>30-03-2022 09:24</t>
-  </si>
-  <si>
-    <t>30-03-2022 09:11</t>
-  </si>
-  <si>
-    <t>30-03-2022 09:07</t>
+    <t>When Tesla beat other automobile companies, Elon dance like this. @elonmusk #ElonMusk #Tesla #Musk #TSLA https://t.co/oz9NxjjPEz</t>
+  </si>
+  <si>
+    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
+https://t.co/XThns6nB6u</t>
+  </si>
+  <si>
+    <t>Every address that is sent too late, gets their BTC immediately sent back #eth #tsla #shib
+https://t.co/NyzrSmmfRz</t>
+  </si>
+  <si>
+    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
+https://t.co/8cGksFdIFn</t>
+  </si>
+  <si>
+    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/Vi9mCR11Q1</t>
+  </si>
+  <si>
+    <t>Every address that is sent too late, gets their BTC immediately sent back #eth #tsla #shib
+https://t.co/4kDOw3ad8Q</t>
+  </si>
+  <si>
+    <t>YWautoparts NEW product-Vehicle to load #TSLA #BDY #NIO #V2L #EVCHARGER #HYUNDAI https://t.co/6dVgzjOb11</t>
+  </si>
+  <si>
+    <t>FSD Update feels very human like. #TSLA https://t.co/o7nimnQ3yt</t>
+  </si>
+  <si>
+    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
+https://t.co/QPa7wuLsAJ</t>
+  </si>
+  <si>
+    <t>Why wait till next week what #tsla can do in a day 🚀⛽️ https://t.co/dVf1ELdnvg</t>
+  </si>
+  <si>
+    <t>Check out my #TSLA analysis on @TradingView: https://t.co/bjoLWuxUt5 
+Indicators I commonly use.
+1. T-Line Candles[CW_Trades]
+2. EMA: 8,21,55,100,200,*400
+3. VWAP - Volume Weighted Average Price
+4. RSI - Relative Strength Index
+5. MACD - Moving Average Convergence Divergence</t>
+  </si>
+  <si>
+    <t>Check out my #TSLA analysis on @TradingView: https://t.co/pegc0a1lQx 
+Recap: TSLA bounced off 200ema, volume came, followed by price action, broke out of previous resistance, took the trade. peaked 13% profit took it at 6%.</t>
+  </si>
+  <si>
+    <t>Every address that is sent too late, gets their BTC immediately sent back #eth #tsla #shib
+https://t.co/MUqPCNrOOD</t>
+  </si>
+  <si>
+    <t>I received this(0.5BTC) amount on my #Uphold wallet. It works! #btc #eth $dogecoin #tsla
+https://t.co/kcbjMuHTvK</t>
+  </si>
+  <si>
+    <t>I received this(5eth) amount on my #Uphold wallet. It works! #btc #eth $dogecoin #tsla
+https://t.co/kcbjMuHTvK</t>
+  </si>
+  <si>
+    <t>@elonmusk @BillyM2k A lot of tendies providable by this end boss.
+$AMC is about to spring squeeze possibly tomorrow. Our end boss is #shitadel, #susqueshit, #simpleshit
+Let's make it happen 4 #change and millions of potential new #TSLA owner. 💪😎 https://t.co/92UXOtGK61</t>
+  </si>
+  <si>
+    <t>$TSLA seeing sustained chatter on wallstreetbets over the last few days_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #trading https://t.co/iLHyafKAO4</t>
+  </si>
+  <si>
+    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
+https://t.co/tJhgG47quR</t>
+  </si>
+  <si>
+    <t>Current position #tsla #OptionsTrading https://t.co/IXX0kNL9VZ</t>
+  </si>
+  <si>
+    <t>$TSLA set up on the hourly chart. Important Levels to get past for upside would start with 1106, then 1113-1115 area and if we get past that room to test 1124.6 high. #SPY #TSLA  #markets #DayTrading https://t.co/9NJR8DFVOf</t>
+  </si>
+  <si>
+    <t>https://t.co/LX6FXA7AQ2 - Tesla Stock “Going Significantly Lower” Says Bear 🤡
+NEW
+$TSLA #Tesla #TSLA #TeslaStock #ElonMusk https://t.co/oAZUz2vQmM</t>
+  </si>
+  <si>
+    <t>Telsa⚡️: Will Stock Split Mirror 2020🚀
+ #TSLA @stevenmarkryan 
+2020
+8/11:  $1,374 Pre-Split
+8/11:  $1,463 +6% PostNews
+8/28: $2,213 +51% close
+8/31 : $  442 5:1 Split
+8/31 : $  498 +12% close
+2022
+3/25: $1,010 Pre-Split
+3/28: $1,091 +8% PostNews
+⭐️TSLA Secured Growth &amp;amp; Split https://t.co/d17BcwiuHK</t>
+  </si>
+  <si>
+    <t>$TSLA #TSLA looks strong looking like its on the way to test $1400.00
+ @TradingView: https://t.co/F2utr6Nn22</t>
+  </si>
+  <si>
+    <t>@elonmusk  Need Passes for “ CYBER RODEO “ Please …… #CyberRodeo #elonamusk #texasgigafactory #Tesla #TSLA #SpaceX #Tesla #Elon #FSDBeta https://t.co/i7qglhgNNx</t>
+  </si>
+  <si>
+    <t>@Tesla @elonmusk Why can I not access the Tesla site? It keeps telling me Access Denied…
+#Tesla #ElonMusk #TSLA</t>
+  </si>
+  <si>
+    <t>@garyblack00 at this point nothing surprises me no more. ill just keep adding more #tsla shares</t>
+  </si>
+  <si>
+    <t>$TSLA #TSLA Ascending triangle on the monthly chart. 
+April is the 3rd best performing month of the year since the IPO in 2010 with a 64% win rate. https://t.co/IeUNZi0X3g</t>
+  </si>
+  <si>
+    <t>$TSLA #TSLA failed to break R2 pivot $1119.75 on several attempts. Bearish divergence with a 9 count today. 
+If PA opens &amp;amp; stays below W-VWAP $1091.74, then possibly pushed lower to test R1 pivot $1065.20 IMO. 
+Gap still needs to be resolved near $1K (ideal move).
+#stocks https://t.co/TZhGdOHc7s</t>
+  </si>
+  <si>
+    <t>@jasondebolt What is your goal to do with your wealth from #Tsla?</t>
+  </si>
+  <si>
+    <t>@wyldeAF @jasondebolt Same here. A majority of my coworkers as well. There is no second best! #tsla</t>
+  </si>
+  <si>
+    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/98lyq3evGq</t>
+  </si>
+  <si>
+    <t>The Big Five #FAANG Stock and Sector Service is now posted for Wednesday #AMZN #AAPL #FB #NFLX #TSLA #GOOGL and  Sector Funds - #IBB #IYR #XLE #XLE #XLF #XLK #XRT    (link: https://t.co/bihMz399my)   #trading #investing #FinancialFreedom https://t.co/xAPMeXgV44</t>
+  </si>
+  <si>
+    <t>Tesla ⚡️: Starship, 4680 Battery &amp;amp; Positive NHTSA Updates!
+#TheTeslaSpace #TSLA 
+• FAA Pushed Starship to 4/29
+• New 4680 Patten Released
+• Significant Faster Production
+• NHTSA Increase Penalties That will Generate More Regulatory Credits for Tesla 
+https://t.co/9H5nNKHRRK https://t.co/iqvryquOPx</t>
+  </si>
+  <si>
+    <t>Posted Daily Analyses/Updates:
+#SP500 #SPX 
+#VIX $VIX
+#Bitcoin #BTCUSD 
+#TSLA $TSLA
+https://t.co/qLx4srPGAT
+https://t.co/6ISQ7l9Zro
+https://t.co/ZGX5F02AoT
+https://t.co/nU40kNanGt
+https://t.co/5V41NUfCij
+Alerts:
+#gold $GLD
+#silver $SLV
+https://t.co/XHPxshnZuM</t>
+  </si>
+  <si>
+    <t>Heavy #Options Flow &amp;gt; $500K – End of day Fat Prints 
+$TSLA #TSLA 1150C 4-1   --&amp;gt;&amp;gt;  $19 MIL. PRINT
+$AMD #AMD 127C 4-1       --&amp;gt;&amp;gt;  $800k   PRINT
+$DDOG #DDOG 160C 5-20 --&amp;gt;&amp;gt; 7.8 MIL. PRINT
+Game changer Data courtesy of @chatterQuant 
+Source: https://t.co/ug9CyDpSas https://t.co/5fjhyvXgDd</t>
+  </si>
+  <si>
+    <t>What is Twitter talking about ?
+#TSLA #AAPL #MU #AMZN #AMC #FB #QQQ #PYPL
+Source: https://t.co/ug9CyDpSas https://t.co/wPW6txHTCD</t>
+  </si>
+  <si>
+    <t>@hershohm @SawyerMerritt Very real possibility. #TSLA https://t.co/51Q9dLHn57</t>
+  </si>
+  <si>
+    <t>$TSLA - Baglino Andrew D sold 7000.0 shares of Common Stock worth $3,947,020.00 in 2 transaction(s) on 2022-03-28  #TSLA</t>
+  </si>
+  <si>
+    <t>The Market's Beginning To Take MULN STOCK Seriously. 100% gains incoming... https://t.co/7Gf9zj2zgi via @YouTube #muln #MULNSQUEEZE #mulnarmy #mulnapes #stocks #stockmarket #NASDAQ100 #nasdaq #wallstreetbets #WallStreet #tsla #tesla</t>
+  </si>
+  <si>
+    <t>It’s @elonmusk though that gives me anxiety &amp;amp; he’s pretty cute what if I giggle…or mess up &amp;amp; call him dude or bro? God forbid I mention @JeffBezos *trust me I’ve heard stories* anyway @elonmusk I’m pretty sleepy &amp;amp; about to take a nap congrats on a marvelous Q1 #TSLA https://t.co/EZnWvUGpqm</t>
+  </si>
+  <si>
+    <t>#Tesla #Tsla #Teslastock 
+In a stock split the number of outstanding shares increases and the price per share decreases proportionately, while the market capitalization and the value of the company do not change. https://t.co/xIRjp5YpsY</t>
+  </si>
+  <si>
+    <t>My co-worker is now looking and reading more about finance management, trading and investing (stocks and crypto) for a target financial stability when he retires from the Military 💪💪. It feels good to be a positive influence👊. You? how did your day went today? #HYMC #TSLA #CEI</t>
+  </si>
+  <si>
+    <t>Our new car has arrived! #TSLA #zeroemmissions @ Barrie, Ontario https://t.co/rpZ7uYLhdL</t>
+  </si>
+  <si>
+    <t>#Tesla #Tsla #Teslastock 
+     Why Is TESLA Splitting ?
+1.  Share Affordability
+2. Improve Trading Liquidity
+     Why Is Share Affordability
+Important For Tesla As A Company ?
+Just So You Know...
+Company Berkshire Hathaway, which hasn't ever had a stock split in its history.</t>
+  </si>
+  <si>
+    <t>$TSLA working its way into the top 10 most mentioned on wallstreetbets over the last 7 days_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #investors https://t.co/AL16lqrvvd</t>
+  </si>
+  <si>
+    <t>https://t.co/6rXZFDtprv
+Streaming today’s Stock Market recap. Everyone welcome to join and ask questions. 
+#SPY #TSLA $MULN</t>
+  </si>
+  <si>
+    <t>I jumped on #Tsla at the right time.</t>
+  </si>
+  <si>
+    <t>$TSLA seeing an uptick in chatter on wallstreetbets over the last 24 hours_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #investing https://t.co/1OSL323qEa</t>
+  </si>
+  <si>
+    <t>New to Finance Twitter, what account should I follow? #StockMarket #Investing #Finance #SP500 #NASDAQ #TSLA #MSFT #AAPL #FB #AMZN #BA #Crypto #Coinbase</t>
+  </si>
+  <si>
+    <t>LIMITED TIME OFFER: Get 5 FREE stocks valued up to $9,600 by opening &amp;amp; funding a #Webull brokerage account! Get started &amp;gt; #BTC #MMAT #Zilliqa
+#TSLA #YOMTVRaps #HipHop #Verzuz #NFT #Stocks #Stockmarket #NFTCommunity #CarlosEMendez https://t.co/YqRmgEv99k https://t.co/1BAMscYwTA</t>
+  </si>
+  <si>
+    <t>31-03-2022 08:33</t>
+  </si>
+  <si>
+    <t>31-03-2022 08:25</t>
+  </si>
+  <si>
+    <t>31-03-2022 08:10</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:55</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:53</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:45</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:42</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:36</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:29</t>
+  </si>
+  <si>
+    <t>31-03-2022 07:17</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:56</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:48</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:40</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:30</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:25</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:20</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:09</t>
+  </si>
+  <si>
+    <t>31-03-2022 05:05</t>
+  </si>
+  <si>
+    <t>31-03-2022 04:25</t>
+  </si>
+  <si>
+    <t>31-03-2022 04:19</t>
+  </si>
+  <si>
+    <t>31-03-2022 04:15</t>
+  </si>
+  <si>
+    <t>31-03-2022 03:56</t>
+  </si>
+  <si>
+    <t>31-03-2022 02:59</t>
+  </si>
+  <si>
+    <t>31-03-2022 02:47</t>
+  </si>
+  <si>
+    <t>31-03-2022 02:44</t>
+  </si>
+  <si>
+    <t>31-03-2022 02:41</t>
+  </si>
+  <si>
+    <t>31-03-2022 02:28</t>
+  </si>
+  <si>
+    <t>31-03-2022 01:58</t>
+  </si>
+  <si>
+    <t>31-03-2022 01:49</t>
+  </si>
+  <si>
+    <t>31-03-2022 01:23</t>
+  </si>
+  <si>
+    <t>31-03-2022 01:14</t>
+  </si>
+  <si>
+    <t>31-03-2022 01:01</t>
+  </si>
+  <si>
+    <t>31-03-2022 00:24</t>
+  </si>
+  <si>
+    <t>31-03-2022 00:12</t>
+  </si>
+  <si>
+    <t>31-03-2022 00:08</t>
+  </si>
+  <si>
+    <t>30-03-2022 23:19</t>
+  </si>
+  <si>
+    <t>30-03-2022 23:17</t>
+  </si>
+  <si>
+    <t>30-03-2022 22:33</t>
+  </si>
+  <si>
+    <t>30-03-2022 22:32</t>
+  </si>
+  <si>
+    <t>30-03-2022 21:44</t>
+  </si>
+  <si>
+    <t>30-03-2022 21:19</t>
+  </si>
+  <si>
+    <t>30-03-2022 21:14</t>
+  </si>
+  <si>
+    <t>30-03-2022 21:11</t>
+  </si>
+  <si>
+    <t>30-03-2022 21:08</t>
+  </si>
+  <si>
+    <t>30-03-2022 20:58</t>
+  </si>
+  <si>
+    <t>30-03-2022 20:50</t>
+  </si>
+  <si>
+    <t>30-03-2022 20:47</t>
+  </si>
+  <si>
+    <t>30-03-2022 20:40</t>
+  </si>
+  <si>
+    <t>30-03-2022 20:28</t>
+  </si>
+  <si>
+    <t>13-11-2021 19:14</t>
+  </si>
+  <si>
+    <t>25-02-2010 05:59</t>
+  </si>
+  <si>
+    <t>04-08-2017 02:58</t>
+  </si>
+  <si>
+    <t>08-04-2021 09:31</t>
+  </si>
+  <si>
+    <t>28-11-2020 04:42</t>
+  </si>
+  <si>
+    <t>30-08-2011 12:26</t>
+  </si>
+  <si>
+    <t>30-09-2017 19:06</t>
+  </si>
+  <si>
+    <t>31-10-2015 10:02</t>
+  </si>
+  <si>
+    <t>08-01-2020 17:10</t>
+  </si>
+  <si>
+    <t>22-03-2022 20:47</t>
+  </si>
+  <si>
+    <t>07-01-2022 06:16</t>
+  </si>
+  <si>
+    <t>14-04-2009 23:28</t>
+  </si>
+  <si>
+    <t>17-12-2021 04:44</t>
+  </si>
+  <si>
+    <t>17-03-2021 13:22</t>
+  </si>
+  <si>
+    <t>29-05-2014 05:06</t>
+  </si>
+  <si>
+    <t>13-10-2021 02:40</t>
+  </si>
+  <si>
+    <t>13-02-2017 20:51</t>
+  </si>
+  <si>
+    <t>19-07-2017 19:21</t>
+  </si>
+  <si>
+    <t>10-12-2016 04:42</t>
+  </si>
+  <si>
+    <t>22-06-2020 00:03</t>
+  </si>
+  <si>
+    <t>24-10-2020 11:31</t>
+  </si>
+  <si>
+    <t>01-09-2011 09:24</t>
+  </si>
+  <si>
+    <t>24-04-2021 05:45</t>
+  </si>
+  <si>
+    <t>19-01-2017 03:39</t>
+  </si>
+  <si>
+    <t>09-07-2021 16:16</t>
+  </si>
+  <si>
+    <t>23-11-2021 02:22</t>
+  </si>
+  <si>
+    <t>18-01-2017 02:58</t>
   </si>
   <si>
     <t>28-09-2021 20:44</t>
   </si>
   <si>
-    <t>01-04-2020 23:46</t>
-  </si>
-  <si>
-    <t>18-12-2012 19:49</t>
-  </si>
-  <si>
-    <t>24-03-2022 02:51</t>
-  </si>
-  <si>
-    <t>10-10-2017 18:17</t>
-  </si>
-  <si>
-    <t>07-11-2016 06:50</t>
-  </si>
-  <si>
-    <t>29-08-2017 00:33</t>
-  </si>
-  <si>
-    <t>11-01-2022 17:24</t>
-  </si>
-  <si>
-    <t>08-06-2018 18:47</t>
-  </si>
-  <si>
-    <t>06-06-2020 21:28</t>
-  </si>
-  <si>
-    <t>09-11-2020 01:03</t>
-  </si>
-  <si>
-    <t>19-01-2014 09:15</t>
-  </si>
-  <si>
-    <t>23-03-2009 01:46</t>
-  </si>
-  <si>
-    <t>27-03-2018 02:20</t>
-  </si>
-  <si>
-    <t>05-03-2022 05:46</t>
-  </si>
-  <si>
-    <t>21-11-2020 19:42</t>
-  </si>
-  <si>
-    <t>03-04-2015 18:06</t>
-  </si>
-  <si>
-    <t>07-08-2018 06:16</t>
-  </si>
-  <si>
-    <t>17-09-2011 19:24</t>
-  </si>
-  <si>
-    <t>22-03-2022 02:32</t>
-  </si>
-  <si>
-    <t>04-03-2009 21:58</t>
-  </si>
-  <si>
-    <t>15-03-2015 17:44</t>
-  </si>
-  <si>
-    <t>25-08-2009 00:39</t>
-  </si>
-  <si>
-    <t>29-05-2020 04:24</t>
-  </si>
-  <si>
-    <t>24-12-2020 22:28</t>
-  </si>
-  <si>
-    <t>15-04-2016 14:42</t>
-  </si>
-  <si>
-    <t>11-01-2011 17:17</t>
-  </si>
-  <si>
-    <t>12-08-2021 00:00</t>
-  </si>
-  <si>
-    <t>24-03-2022 14:41</t>
-  </si>
-  <si>
-    <t>04-08-2017 02:58</t>
-  </si>
-  <si>
-    <t>07-11-2010 00:01</t>
-  </si>
-  <si>
-    <t>26-01-2012 01:45</t>
-  </si>
-  <si>
-    <t>14-07-2021 15:05</t>
-  </si>
-  <si>
-    <t>08-01-2020 17:10</t>
-  </si>
-  <si>
-    <t>24-06-2015 14:30</t>
-  </si>
-  <si>
-    <t>29-09-2020 16:38</t>
-  </si>
-  <si>
-    <t>28-07-2009 02:25</t>
-  </si>
-  <si>
-    <t>23-04-2010 17:28</t>
-  </si>
-  <si>
-    <t>04-09-2018 16:36</t>
-  </si>
-  <si>
-    <t>24-05-2010 19:33</t>
-  </si>
-  <si>
-    <t>29-03-2022 02:15</t>
-  </si>
-  <si>
-    <t>04-12-2019 10:53</t>
-  </si>
-  <si>
-    <t>15-10-2011 23:44</t>
-  </si>
-  <si>
-    <t>03-04-2018 06:05</t>
-  </si>
-  <si>
-    <t>29-01-2021 14:40</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [22, 27]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [58, 63]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [73, 78]}, {'text': 'ES', 'indices': [100, 103]}, {'text': 'NASDAQ', 'indices': [105, 112]}, {'text': 'DXY', 'indices': [114, 118]}, {'text': 'Gold', 'indices': [120, 125]}, {'text': 'Silver', 'indices': [127, 134]}, {'text': 'CrudeOil', 'indices': [136, 145]}, {'text': 'Soybeans', 'indices': [150, 159]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'spy', 'indices': [186, 190]}, {'text': 'tsla', 'indices': [191, 196]}, {'text': 'minerals', 'indices': [197, 206]}, {'text': 'vale', 'indices': [207, 212]}, {'text': 'copper', 'indices': [213, 220]}, {'text': 'uraniumsqueeze', 'indices': [221, 236]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tesla', 'indices': [55, 61]}, {'text': 'tsla', 'indices': [62, 67]}, {'text': 'teslastock', 'indices': [68, 79]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [46, 51]}, {'text': 'Doge', 'indices': [52, 57]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [52, 57]}, {'text': 'pltr', 'indices': [58, 63]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [0, 5]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [40, 45]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [46, 51]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [144, 149]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'AMC', 'indices': [28, 32]}, {'text': 'GME', 'indices': [33, 37]}, {'text': 'TLRY', 'indices': [38, 43]}, {'text': 'TSLA', 'indices': [44, 49]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [0, 5]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [47, 52]}, {'text': 'InvexGlobal', 'indices': [53, 65]}, {'text': 'OptionsTrading', 'indices': [66, 81]}, {'text': 'Options', 'indices': [82, 90]}, {'text': 'NASDAQ', 'indices': [91, 98]}, {'text': 'NYSE', 'indices': [99, 104]}, {'text': 'trading', 'indices': [105, 113]}, {'text': 'stocks', 'indices': [114, 121]}, {'text': 'daytrading', 'indices': [122, 133]}, {'text': 'market', 'indices': [134, 141]}, {'text': 'investors', 'indices': [142, 152]}, {'text': 'USA', 'indices': [153, 157]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [66, 71]}, {'text': 'tesla', 'indices': [72, 78]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [62, 67]}, {'text': 'TESLA', 'indices': [68, 74]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [73, 78]}, {'text': 'NVDA', 'indices': [114, 119]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'ElonMusk', 'indices': [50, 59]}, {'text': 'TSLA', 'indices': [60, 65]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'battery', 'indices': [137, 145]}, {'text': 'Tesla', 'indices': [205, 211]}, {'text': 'TSLA', 'indices': [222, 227]}, {'text': 'Investor', 'indices': [228, 237]}, {'text': 'EVs', 'indices': [238, 242]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [44, 50]}, {'text': 'solar', 'indices': [84, 90]}, {'text': 'renewableenergy', 'indices': [146, 162]}, {'text': 'renewables', 'indices': [163, 174]}, {'text': 'tsla', 'indices': [175, 180]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [23, 28]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'nio', 'indices': [0, 4]}, {'text': 'expv', 'indices': [18, 23]}, {'text': 'tsla', 'indices': [93, 98]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'spy', 'indices': [0, 4]}, {'text': 'SPX', 'indices': [10, 14]}, {'text': 'QQQ', 'indices': [25, 29]}, {'text': 'ES_F', 'indices': [30, 35]}, {'text': 'NQ_F', 'indices': [42, 47]}, {'text': 'VIX', 'indices': [59, 63]}, {'text': 'AAPL', 'indices': [70, 75]}, {'text': 'MSFT', 'indices': [82, 87]}, {'text': 'GOOGL', 'indices': [95, 101]}, {'text': 'AMZN', 'indices': [108, 113]}, {'text': 'FB', 'indices': [118, 121]}, {'text': 'TLT', 'indices': [127, 131]}, {'text': 'ARKK', 'indices': [144, 149]}, {'text': 'TSLA', 'indices': [156, 161]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [0, 5]}, {'text': 'VALE', 'indices': [54, 59]}, {'text': 'TSLA', 'indices': [180, 185]}, {'text': 'BHP', 'indices': [228, 232]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [55, 60]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Natural_Gas', 'indices': [29, 41]}, {'text': 'Crude_Oil', 'indices': [42, 52]}, {'text': 'Gold', 'indices': [53, 58]}, {'text': 'Silver', 'indices': [59, 66]}, {'text': 'TSX', 'indices': [67, 71]}, {'text': 'SPY', 'indices': [72, 76]}, {'text': 'QQQ', 'indices': [77, 81]}, {'text': 'TSLA', 'indices': [82, 87]}, {'text': 'SHOP', 'indices': [88, 93]}, {'text': 'Trading', 'indices': [97, 105]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'CanadaNickel', 'indices': [86, 99]}, {'text': 'SudburyTwoPointO', 'indices': [101, 118]}, {'text': 'NetZeroNickel', 'indices': [119, 133]}, {'text': 'TM', 'indices': [135, 138]}, {'text': 'Nickel', 'indices': [140, 147]}, {'text': 'EV', 'indices': [178, 181]}, {'text': 'BatteryMetals', 'indices': [182, 196]}, {'text': 'Reddit', 'indices': [199, 206]}, {'text': 'TSLA', 'indices': [207, 212]}, {'text': 'ESG', 'indices': [213, 217]}, {'text': 'Mining', 'indices': [218, 225]}, {'text': 'ElonMusk', 'indices': [226, 235]}, {'text': 'Glencore', 'indices': [237, 246]}, {'text': 'BHP', 'indices': [247, 251]}, {'text': 'Vale', 'indices': [252, 257]}, {'text': 'Timmins', 'indices': [258, 266]}, {'text': 'Canada', 'indices': [267, 274]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [54, 59]}, {'text': 'cleanenergy', 'indices': [60, 72]}, {'text': 'energy', 'indices': [73, 80]}, {'text': 'fossilfuels', 'indices': [81, 93]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [31, 36]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'OptionsTrading', 'indices': [234, 249]}, {'text': 'TSLA', 'indices': [250, 255]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'BNTX', 'indices': [25, 30]}, {'text': 'CHWY', 'indices': [36, 41]}, {'text': 'LULU', 'indices': [49, 54]}, {'text': 'TSLA', 'indices': [59, 64]}, {'text': 'fypシ', 'indices': [91, 96]}, {'text': 'tiktok', 'indices': [97, 104]}, {'text': 'viral', 'indices': [105, 111]}, {'text': 'stockmarket', 'indices': [112, 124]}, {'text': 'stocks', 'indices': [125, 132]}, {'text': 'tranding', 'indices': [133, 142]}, {'text': 'fanpage', 'indices': [143, 151]}, {'text': 'BTCUSD', 'indices': [152, 159]}, {'text': 'DowJones', 'indices': [160, 169]}, {'text': 'Futures', 'indices': [170, 178]}, {'text': 'forextrading', 'indices': [179, 192]}, {'text': 'NASDAQ', 'indices': [193, 200]}, {'text': 'GameStop', 'indices': [201, 210]}, {'text': 'AMCSTOCK', 'indices': [211, 220]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [0, 5]}, {'text': 'CEDEAR', 'indices': [8, 15]}, {'text': 'EEUU', 'indices': [51, 56]}, {'text': 'tecnología', 'indices': [57, 68]}, {'text': 'research', 'indices': [69, 78]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [21, 26]}, {'text': 'AMC', 'indices': [27, 31]}, {'text': 'CRWD', 'indices': [32, 37]}, {'text': 'TAN', 'indices': [38, 42]}, {'text': 'W', 'indices': [43, 45]}, {'text': 'StocksToWatch', 'indices': [74, 88]}, {'text': 'DayTrading', 'indices': [89, 100]}, {'text': 'OptionsTrading', 'indices': [101, 116]}, {'text': 'Options', 'indices': [117, 125]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [9, 14]}]</t>
+    <t>25-08-2020 16:39</t>
+  </si>
+  <si>
+    <t>28-05-2020 02:39</t>
+  </si>
+  <si>
+    <t>30-12-2019 01:46</t>
+  </si>
+  <si>
+    <t>25-10-2020 07:23</t>
+  </si>
+  <si>
+    <t>31-05-2010 16:38</t>
+  </si>
+  <si>
+    <t>30-03-2022 17:05</t>
+  </si>
+  <si>
+    <t>29-01-2013 11:00</t>
+  </si>
+  <si>
+    <t>[{'text': 'ElonMusk', 'indices': [76, 85]}, {'text': 'Tesla', 'indices': [86, 92]}, {'text': 'Musk', 'indices': [93, 98]}, {'text': 'TSLA', 'indices': [99, 104]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'btc', 'indices': [25, 29]}, {'text': 'tsla', 'indices': [58, 63]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'eth', 'indices': [74, 78]}, {'text': 'tsla', 'indices': [79, 84]}, {'text': 'shib', 'indices': [85, 90]}]</t>
   </si>
   <si>
     <t>[{'text': 'tesla', 'indices': [26, 32]}, {'text': 'tsla', 'indices': [33, 38]}, {'text': 'stock', 'indices': [39, 45]}, {'text': 'stockmarket', 'indices': [46, 58]}, {'text': 'options', 'indices': [59, 67]}, {'text': 'money', 'indices': [68, 74]}, {'text': 'cars', 'indices': [75, 80]}, {'text': 'tech', 'indices': [81, 86]}, {'text': 'technology', 'indices': [87, 98]}]</t>
   </si>
   <si>
-    <t>[{'text': 'Tesla', 'indices': [0, 6]}, {'text': 'tsla', 'indices': [7, 12]}, {'text': 'split', 'indices': [42, 48]}, {'text': 'Wedbush', 'indices': [96, 104]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [9, 15]}, {'text': 'Model2', 'indices': [16, 23]}, {'text': 'electricvehicle', 'indices': [134, 150]}, {'text': 'tsla', 'indices': [155, 160]}, {'text': 'elon', 'indices': [161, 166]}, {'text': 'elonmusk', 'indices': [167, 176]}, {'text': 'electriccar', 'indices': [177, 189]}, {'text': 'cars', 'indices': [190, 195]}, {'text': 'carnews', 'indices': [196, 204]}, {'text': 'driving', 'indices': [205, 213]}]</t>
+    <t>[{'text': 'TSLA', 'indices': [40, 45]}, {'text': 'BDY', 'indices': [46, 50]}, {'text': 'NIO', 'indices': [51, 55]}, {'text': 'V2L', 'indices': [56, 60]}, {'text': 'EVCHARGER', 'indices': [61, 71]}, {'text': 'HYUNDAI', 'indices': [72, 80]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [34, 39]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [29, 34]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [13, 18]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Uphold', 'indices': [37, 44]}, {'text': 'btc', 'indices': [63, 67]}, {'text': 'eth', 'indices': [68, 72]}, {'text': 'tsla', 'indices': [83, 88]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Uphold', 'indices': [35, 42]}, {'text': 'btc', 'indices': [61, 65]}, {'text': 'eth', 'indices': [66, 70]}, {'text': 'tsla', 'indices': [81, 86]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'shitadel', 'indices': [133, 142]}, {'text': 'susqueshit', 'indices': [144, 155]}, {'text': 'simpleshit', 'indices': [157, 168]}, {'text': 'change', 'indices': [192, 199]}, {'text': 'TSLA', 'indices': [230, 235]}]</t>
   </si>
   <si>
     <t>[{'text': 'tsla', 'indices': [102, 107]}, {'text': 'wallstreetbets', 'indices': [111, 126]}, {'text': 'trading', 'indices': [128, 136]}]</t>
   </si>
   <si>
-    <t>[{'text': 'tsla', 'indices': [198, 203]}, {'text': 'tesla', 'indices': [204, 210]}, {'text': 'Q12022', 'indices': [211, 218]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [18, 23]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [79, 84]}, {'text': 'teslastock', 'indices': [85, 96]}, {'text': 'StockMarket', 'indices': [97, 109]}, {'text': 'StockSplit', 'indices': [110, 121]}, {'text': 'fintwit', 'indices': [122, 130]}, {'text': 'FinTwitt', 'indices': [131, 140]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TESLA', 'indices': [0, 6]}, {'text': 'TSLA', 'indices': [7, 12]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'sp500', 'indices': [190, 196]}, {'text': 'Bitcoin', 'indices': [197, 205]}, {'text': 'TSLA', 'indices': [224, 229]}, {'text': 'NASDAQ', 'indices': [230, 237]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLAQ', 'indices': [123, 129]}, {'text': 'TSLA', 'indices': [130, 135]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'BTC', 'indices': [0, 4]}, {'text': 'TSLA', 'indices': [5, 10]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [14, 19]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [3, 8]}, {'text': 'teslastock', 'indices': [51, 62]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [140, 145]}, {'text': 'btc', 'indices': [224, 228]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Elonmusk', 'indices': [12, 21]}, {'text': 'tsla', 'indices': [22, 27]}, {'text': 'audi', 'indices': [28, 33]}, {'text': 'volkswagen', 'indices': [34, 45]}, {'text': 'porsche', 'indices': [46, 54]}, {'text': 'mercedes', 'indices': [55, 64]}, {'text': 'panasonic', 'indices': [65, 75]}, {'text': 'varta', 'indices': [76, 82]}, {'text': 'bmw', 'indices': [83, 87]}, {'text': 'recycling', 'indices': [88, 98]}, {'text': 'recycle', 'indices': [99, 107]}, {'text': 'electricvehicle', 'indices': [108, 124]}, {'text': 'batteries', 'indices': [125, 135]}]</t>
+    <t>[{'text': 'tsla', 'indices': [17, 22]}, {'text': 'OptionsTrading', 'indices': [23, 38]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'SPY', 'indices': [167, 171]}, {'text': 'TSLA', 'indices': [172, 177]}, {'text': 'markets', 'indices': [179, 187]}, {'text': 'DayTrading', 'indices': [188, 199]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [90, 96]}, {'text': 'TSLA', 'indices': [97, 102]}, {'text': 'TeslaStock', 'indices': [103, 114]}, {'text': 'ElonMusk', 'indices': [115, 124]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [40, 45]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [6, 11]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'CyberRodeo', 'indices': [53, 64]}, {'text': 'elonamusk', 'indices': [65, 75]}, {'text': 'texasgigafactory', 'indices': [76, 93]}, {'text': 'Tesla', 'indices': [94, 100]}, {'text': 'TSLA', 'indices': [101, 106]}, {'text': 'SpaceX', 'indices': [107, 114]}, {'text': 'Tesla', 'indices': [115, 121]}, {'text': 'Elon', 'indices': [122, 127]}, {'text': 'FSDBeta', 'indices': [128, 136]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [89, 95]}, {'text': 'ElonMusk', 'indices': [96, 105]}, {'text': 'TSLA', 'indices': [106, 111]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [83, 88]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'stocks', 'indices': [272, 279]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tsla', 'indices': [59, 64]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [94, 99]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'FAANG', 'indices': [13, 19]}, {'text': 'AMZN', 'indices': [73, 78]}, {'text': 'AAPL', 'indices': [79, 84]}, {'text': 'FB', 'indices': [85, 88]}, {'text': 'NFLX', 'indices': [89, 94]}, {'text': 'TSLA', 'indices': [95, 100]}, {'text': 'GOOGL', 'indices': [101, 107]}, {'text': 'IBB', 'indices': [128, 132]}, {'text': 'IYR', 'indices': [133, 137]}, {'text': 'XLE', 'indices': [138, 142]}, {'text': 'XLE', 'indices': [143, 147]}, {'text': 'XLF', 'indices': [148, 152]}, {'text': 'XLK', 'indices': [153, 157]}, {'text': 'XRT', 'indices': [158, 162]}, {'text': 'trading', 'indices': [200, 208]}, {'text': 'investing', 'indices': [209, 219]}, {'text': 'FinancialFreedom', 'indices': [220, 237]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TheTeslaSpace', 'indices': [63, 77]}, {'text': 'TSLA', 'indices': [78, 83]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'SP500', 'indices': [31, 37]}, {'text': 'SPX', 'indices': [38, 42]}, {'text': 'VIX', 'indices': [44, 48]}, {'text': 'Bitcoin', 'indices': [54, 62]}, {'text': 'BTCUSD', 'indices': [63, 70]}, {'text': 'TSLA', 'indices': [72, 77]}, {'text': 'gold', 'indices': [214, 219]}, {'text': 'silver', 'indices': [225, 232]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Options', 'indices': [6, 14]}, {'text': 'TSLA', 'indices': [64, 69]}, {'text': 'AMD', 'indices': [115, 119]}, {'text': 'DDOG', 'indices': [168, 173]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [33, 38]}, {'text': 'AAPL', 'indices': [39, 44]}, {'text': 'MU', 'indices': [45, 48]}, {'text': 'AMZN', 'indices': [49, 54]}, {'text': 'AMC', 'indices': [55, 59]}, {'text': 'FB', 'indices': [60, 63]}, {'text': 'QQQ', 'indices': [64, 68]}, {'text': 'PYPL', 'indices': [69, 74]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [48, 53]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [115, 120]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'muln', 'indices': [113, 118]}, {'text': 'MULNSQUEEZE', 'indices': [119, 131]}, {'text': 'mulnarmy', 'indices': [132, 141]}, {'text': 'mulnapes', 'indices': [142, 151]}, {'text': 'stocks', 'indices': [152, 159]}, {'text': 'stockmarket', 'indices': [160, 172]}, {'text': 'NASDAQ100', 'indices': [173, 183]}, {'text': 'nasdaq', 'indices': [184, 191]}, {'text': 'wallstreetbets', 'indices': [192, 207]}, {'text': 'WallStreet', 'indices': [208, 219]}, {'text': 'tsla', 'indices': [220, 225]}, {'text': 'tesla', 'indices': [226, 232]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [273, 278]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [0, 6]}, {'text': 'Tsla', 'indices': [7, 12]}, {'text': 'Teslastock', 'indices': [13, 24]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'HYMC', 'indices': [261, 266]}, {'text': 'TSLA', 'indices': [267, 272]}, {'text': 'CEI', 'indices': [273, 277]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [25, 30]}, {'text': 'zeroemmissions', 'indices': [31, 46]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [122, 127]}, {'text': 'wallstreetbets', 'indices': [131, 146]}, {'text': 'investors', 'indices': [148, 158]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'SPY', 'indices': [109, 113]}, {'text': 'TSLA', 'indices': [114, 119]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tsla', 'indices': [12, 17]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [105, 110]}, {'text': 'wallstreetbets', 'indices': [114, 129]}, {'text': 'investing', 'indices': [131, 141]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'StockMarket', 'indices': [54, 66]}, {'text': 'Investing', 'indices': [67, 77]}, {'text': 'Finance', 'indices': [78, 86]}, {'text': 'SP500', 'indices': [87, 93]}, {'text': 'NASDAQ', 'indices': [94, 101]}, {'text': 'TSLA', 'indices': [102, 107]}, {'text': 'MSFT', 'indices': [108, 113]}, {'text': 'AAPL', 'indices': [114, 119]}, {'text': 'FB', 'indices': [120, 123]}, {'text': 'AMZN', 'indices': [124, 129]}, {'text': 'BA', 'indices': [130, 133]}, {'text': 'Crypto', 'indices': [134, 141]}, {'text': 'Coinbase', 'indices': [142, 151]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Webull', 'indices': [85, 92]}, {'text': 'BTC', 'indices': [129, 133]}, {'text': 'MMAT', 'indices': [134, 139]}, {'text': 'Zilliqa', 'indices': [140, 148]}, {'text': 'TSLA', 'indices': [149, 154]}, {'text': 'YOMTVRaps', 'indices': [155, 165]}, {'text': 'HipHop', 'indices': [166, 173]}, {'text': 'Verzuz', 'indices': [174, 181]}, {'text': 'NFT', 'indices': [182, 186]}, {'text': 'Stocks', 'indices': [187, 194]}, {'text': 'Stockmarket', 'indices': [195, 207]}, {'text': 'NFTCommunity', 'indices': [208, 221]}, {'text': 'CarlosEMendez', 'indices': [222, 236]}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +655,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -727,16 +696,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1066,7 +1041,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1078,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1092,22 +1067,22 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>164305</v>
+        <v>1064</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1118,7 +1093,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1891</v>
+        <v>1064</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -1130,10 +1105,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1144,7 +1119,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1064</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -1156,10 +1131,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1170,7 +1145,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>84</v>
+        <v>268</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -1182,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1196,22 +1171,22 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>81</v>
+        <v>1064</v>
       </c>
       <c r="D7" t="s">
         <v>62</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H7" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1222,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -1237,7 +1212,7 @@
         <v>109</v>
       </c>
       <c r="H8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1248,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>748</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -1263,7 +1238,7 @@
         <v>110</v>
       </c>
       <c r="H9" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1274,10 +1249,10 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>37</v>
+        <v>1064</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1286,10 +1261,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1300,10 +1275,10 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1315,7 +1290,7 @@
         <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1326,10 +1301,10 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>823</v>
+        <v>685</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1341,7 +1316,7 @@
         <v>112</v>
       </c>
       <c r="H12" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1352,22 +1327,22 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>164305</v>
+        <v>685</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E13">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1378,10 +1353,10 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>1064</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1390,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1404,10 +1379,10 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>258</v>
+        <v>1064</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1416,10 +1391,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H15" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1430,10 +1405,10 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>1064</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1442,10 +1417,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1456,22 +1431,22 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>4763</v>
+        <v>677</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1482,10 +1457,10 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>35</v>
+        <v>3141</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1494,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1508,10 +1483,10 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>1064</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1520,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H19" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1534,10 +1509,10 @@
         <v>25</v>
       </c>
       <c r="C20">
-        <v>151</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1546,10 +1521,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H20" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1560,48 +1535,48 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <v>196</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H21" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C22">
-        <v>37</v>
+        <v>99654</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1612,10 +1587,10 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1624,10 +1599,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1638,10 +1613,10 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>91</v>
+        <v>809</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1650,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H24" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1664,22 +1639,22 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>208</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H25" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1690,10 +1665,10 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1702,10 +1677,10 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H26" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1716,10 +1691,10 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>863</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1728,10 +1703,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H27" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1742,22 +1717,22 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>2310</v>
+        <v>157483</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E28">
+        <v>19</v>
+      </c>
+      <c r="F28" t="b">
         <v>1</v>
       </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
       <c r="G28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1768,10 +1743,10 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>13150</v>
+        <v>6473</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1780,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H29" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1794,10 +1769,10 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>777</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1806,10 +1781,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H30" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1820,10 +1795,10 @@
         <v>36</v>
       </c>
       <c r="C31">
-        <v>525</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1832,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H31" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1846,10 +1821,10 @@
         <v>37</v>
       </c>
       <c r="C32">
-        <v>71</v>
+        <v>268</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1858,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="H32" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1872,22 +1847,22 @@
         <v>38</v>
       </c>
       <c r="C33">
-        <v>21787</v>
+        <v>2280</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H33" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1898,10 +1873,10 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1910,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H34" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1924,10 +1899,10 @@
         <v>40</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>2099</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1936,10 +1911,10 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H35" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1950,22 +1925,22 @@
         <v>41</v>
       </c>
       <c r="C36">
-        <v>268</v>
+        <v>4245</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H36" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1976,10 +1951,10 @@
         <v>42</v>
       </c>
       <c r="C37">
-        <v>108</v>
+        <v>4245</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1988,10 +1963,10 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H37" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2002,10 +1977,10 @@
         <v>43</v>
       </c>
       <c r="C38">
-        <v>278</v>
+        <v>816</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2014,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H38" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2028,22 +2003,22 @@
         <v>44</v>
       </c>
       <c r="C39">
-        <v>882</v>
+        <v>57</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H39" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2054,10 +2029,10 @@
         <v>45</v>
       </c>
       <c r="C40">
-        <v>3139</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2066,10 +2041,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H40" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2080,22 +2055,22 @@
         <v>46</v>
       </c>
       <c r="C41">
-        <v>3232</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H41" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2106,10 +2081,10 @@
         <v>47</v>
       </c>
       <c r="C42">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2118,10 +2093,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H42" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2132,22 +2107,22 @@
         <v>48</v>
       </c>
       <c r="C43">
-        <v>218586</v>
+        <v>2173</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E43">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H43" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2158,22 +2133,22 @@
         <v>49</v>
       </c>
       <c r="C44">
-        <v>1189</v>
+        <v>83</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H44" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2184,22 +2159,22 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>522</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H45" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2210,10 +2185,10 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>19</v>
+        <v>3141</v>
       </c>
       <c r="D46" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2222,24 +2197,24 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="H46" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C47">
-        <v>22</v>
+        <v>346</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2248,10 +2223,10 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H47" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2262,10 +2237,10 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>9</v>
+        <v>4725</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2274,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="H48" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2288,10 +2263,10 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>156</v>
+        <v>3141</v>
       </c>
       <c r="D49" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2300,10 +2275,10 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="H49" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2314,10 +2289,10 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>646</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2326,10 +2301,10 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H50" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2340,25 +2315,29 @@
         <v>56</v>
       </c>
       <c r="C51">
-        <v>425</v>
+        <v>798</v>
       </c>
       <c r="D51" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H51" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1" location="Tesla%20#TSLA%20#TeslaStock%20#ElonMusk%20https://t.co/oAZUz2vQmM"/>
+    <hyperlink ref="B47" r:id="rId2" location="SPY%20#TSLA%20$MULN"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#feature implemented Tweet Classes
</commit_message>
<xml_diff>
--- a/docs/datasets/tweet_dataset.xlsx
+++ b/docs/datasets/tweet_dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="187">
   <si>
     <t>Tweet</t>
   </si>
@@ -37,603 +37,590 @@
     <t>Hashtags</t>
   </si>
   <si>
-    <t>When Tesla beat other automobile companies, Elon dance like this. @elonmusk #ElonMusk #Tesla #Musk #TSLA https://t.co/oz9NxjjPEz</t>
-  </si>
-  <si>
-    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
-https://t.co/XThns6nB6u</t>
-  </si>
-  <si>
-    <t>Every address that is sent too late, gets their BTC immediately sent back #eth #tsla #shib
-https://t.co/NyzrSmmfRz</t>
-  </si>
-  <si>
-    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
-https://t.co/8cGksFdIFn</t>
-  </si>
-  <si>
-    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/Vi9mCR11Q1</t>
-  </si>
-  <si>
-    <t>Every address that is sent too late, gets their BTC immediately sent back #eth #tsla #shib
-https://t.co/4kDOw3ad8Q</t>
-  </si>
-  <si>
-    <t>YWautoparts NEW product-Vehicle to load #TSLA #BDY #NIO #V2L #EVCHARGER #HYUNDAI https://t.co/6dVgzjOb11</t>
-  </si>
-  <si>
-    <t>FSD Update feels very human like. #TSLA https://t.co/o7nimnQ3yt</t>
-  </si>
-  <si>
-    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
-https://t.co/QPa7wuLsAJ</t>
-  </si>
-  <si>
-    <t>Why wait till next week what #tsla can do in a day 🚀⛽️ https://t.co/dVf1ELdnvg</t>
-  </si>
-  <si>
-    <t>Check out my #TSLA analysis on @TradingView: https://t.co/bjoLWuxUt5 
-Indicators I commonly use.
-1. T-Line Candles[CW_Trades]
-2. EMA: 8,21,55,100,200,*400
-3. VWAP - Volume Weighted Average Price
-4. RSI - Relative Strength Index
-5. MACD - Moving Average Convergence Divergence</t>
-  </si>
-  <si>
-    <t>Check out my #TSLA analysis on @TradingView: https://t.co/pegc0a1lQx 
-Recap: TSLA bounced off 200ema, volume came, followed by price action, broke out of previous resistance, took the trade. peaked 13% profit took it at 6%.</t>
-  </si>
-  <si>
-    <t>Every address that is sent too late, gets their BTC immediately sent back #eth #tsla #shib
-https://t.co/MUqPCNrOOD</t>
-  </si>
-  <si>
-    <t>I received this(0.5BTC) amount on my #Uphold wallet. It works! #btc #eth $dogecoin #tsla
-https://t.co/kcbjMuHTvK</t>
-  </si>
-  <si>
-    <t>I received this(5eth) amount on my #Uphold wallet. It works! #btc #eth $dogecoin #tsla
-https://t.co/kcbjMuHTvK</t>
-  </si>
-  <si>
-    <t>@elonmusk @BillyM2k A lot of tendies providable by this end boss.
-$AMC is about to spring squeeze possibly tomorrow. Our end boss is #shitadel, #susqueshit, #simpleshit
-Let's make it happen 4 #change and millions of potential new #TSLA owner. 💪😎 https://t.co/92UXOtGK61</t>
-  </si>
-  <si>
-    <t>$TSLA seeing sustained chatter on wallstreetbets over the last few days_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #trading https://t.co/iLHyafKAO4</t>
-  </si>
-  <si>
-    <t>Ethereum go slightly up, #btc go please go to the moooon! #tsla
-https://t.co/tJhgG47quR</t>
-  </si>
-  <si>
-    <t>Current position #tsla #OptionsTrading https://t.co/IXX0kNL9VZ</t>
-  </si>
-  <si>
-    <t>$TSLA set up on the hourly chart. Important Levels to get past for upside would start with 1106, then 1113-1115 area and if we get past that room to test 1124.6 high. #SPY #TSLA  #markets #DayTrading https://t.co/9NJR8DFVOf</t>
-  </si>
-  <si>
-    <t>https://t.co/LX6FXA7AQ2 - Tesla Stock “Going Significantly Lower” Says Bear 🤡
+    <t>We wish you more Bitcoins and...healthy fruits in April 😄
+#newmonth #bitcoin #ethereum #btc #satoshi #cryptonews #binance #satoshinakamoto #btcmemes #tsla #wallstreetbets #metaverse #defi #nft #dogecoin https://t.co/gekJIWEp2J</t>
+  </si>
+  <si>
+    <t>@elonmusk @tesla must see 👇
+#tesla #tsla
+@SawyerMerritt
+@WholeMarsBlog 
+@TeslaPodcast 
+@battleangelviv 
+@heydave7 
+@teslaownersSV https://t.co/2N168m6P7U</t>
+  </si>
+  <si>
+    <t>TLRY over $20 than $50 soon next week 💯 💰 🍀 🚀 #Shortsqueeze #LegalizeWeed #Cannabis #Wallstreetbets 🔥#Reddit #Stonks #GME #AMC #TSLA #Elondoge #Bitcoin #Apes #Shib  https://t.co/rLv9QO4x28</t>
+  </si>
+  <si>
+    <t>@TeslaAndDoge I don’t see how #pltr can be the next stonk after #tsla. They’re not B2C, at least not yet.</t>
+  </si>
+  <si>
+    <t>@GordonJohnson19 JUST CHANGED HIS RATING TO BUY #TSLA</t>
+  </si>
+  <si>
+    <t>Now it‘s official that #TSLA is a government protected company https://t.co/tQ5OxOf85T</t>
+  </si>
+  <si>
+    <t>Here’s a group of stocks that have potential upside for a trade. I said trade not investment advice. #GME #AMC  #SNDL  #TSLA  #WISH #JMIA #BIGC.</t>
+  </si>
+  <si>
+    <t>WTF is #TSLA down -24% 
+pre-market ????
+Any specific #Tesla news? https://t.co/ygnahcmuSh</t>
+  </si>
+  <si>
+    <t>$TSLA #TSLA BROKE OUT OF 2 week uptrend &amp;amp; now in a retracing period to test 1075 support level which served as previous support. A bounce off would lead to 1106 resistance and possible 1127.  Break underneath 1075 support and a "fail to retest" would result in a move to 1054. https://t.co/k6e7m5ZIin</t>
+  </si>
+  <si>
+    <t>Thanks to #tsla 🤑⛽️🚀💚 #StocksToBuy  #StockSplit  #stockstowatch #bullsarein #WHALES https://t.co/gP9svWpV7t</t>
+  </si>
+  <si>
+    <t>And then there's even more publicity from the outraged fans of Musk, Tesla or SpaceX.
+Controversy brings publicity.
+#SPACEX, #Tesla, #TSLA, #TSLAQ</t>
+  </si>
+  <si>
+    <t>$TSLA working its way into the top 10 most mentioned on wallstreetbets over the last 24 hours_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #stockmarket https://t.co/Qb543T75lQ</t>
+  </si>
+  <si>
+    <t>This guy had a lot to say about #tsla 🔮⛽️🚀😍 real #stock #shareholders  know the truth behind all this .  @elonmusk  is on another level 🙃 https://t.co/RiePJHDLdK</t>
+  </si>
+  <si>
+    <t>The #StockMarket  is putting a lower price on #tsla  cuz they think this is where the price is yet #tsla is a growing monster that’s out smoking all the car makers. They don’t want to believe the numbers but they don’t lie .  Wait for the big push to come soon 👀⛽️💪🏼</t>
+  </si>
+  <si>
+    <t>@RedTeslaGirl @matthew35746729 @Jefferies @Yahoo @Tesla The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@financiahlth @YouTube The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@eltroglograd @Tesla The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@shanthirex The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@Moshkelgosha_M The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@EXOTICSPEED The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>https://t.co/WUHbGSrydG - Tesla “Defying Gravity” As Karen Attacks &amp;amp; TIME Snubs
 NEW
-$TSLA #Tesla #TSLA #TeslaStock #ElonMusk https://t.co/oAZUz2vQmM</t>
-  </si>
-  <si>
-    <t>Telsa⚡️: Will Stock Split Mirror 2020🚀
- #TSLA @stevenmarkryan 
-2020
-8/11:  $1,374 Pre-Split
-8/11:  $1,463 +6% PostNews
-8/28: $2,213 +51% close
-8/31 : $  442 5:1 Split
-8/31 : $  498 +12% close
-2022
-3/25: $1,010 Pre-Split
-3/28: $1,091 +8% PostNews
-⭐️TSLA Secured Growth &amp;amp; Split https://t.co/d17BcwiuHK</t>
-  </si>
-  <si>
-    <t>$TSLA #TSLA looks strong looking like its on the way to test $1400.00
- @TradingView: https://t.co/F2utr6Nn22</t>
-  </si>
-  <si>
-    <t>@elonmusk  Need Passes for “ CYBER RODEO “ Please …… #CyberRodeo #elonamusk #texasgigafactory #Tesla #TSLA #SpaceX #Tesla #Elon #FSDBeta https://t.co/i7qglhgNNx</t>
-  </si>
-  <si>
-    <t>@Tesla @elonmusk Why can I not access the Tesla site? It keeps telling me Access Denied…
-#Tesla #ElonMusk #TSLA</t>
-  </si>
-  <si>
-    <t>@garyblack00 at this point nothing surprises me no more. ill just keep adding more #tsla shares</t>
-  </si>
-  <si>
-    <t>$TSLA #TSLA Ascending triangle on the monthly chart. 
-April is the 3rd best performing month of the year since the IPO in 2010 with a 64% win rate. https://t.co/IeUNZi0X3g</t>
-  </si>
-  <si>
-    <t>$TSLA #TSLA failed to break R2 pivot $1119.75 on several attempts. Bearish divergence with a 9 count today. 
-If PA opens &amp;amp; stays below W-VWAP $1091.74, then possibly pushed lower to test R1 pivot $1065.20 IMO. 
-Gap still needs to be resolved near $1K (ideal move).
-#stocks https://t.co/TZhGdOHc7s</t>
-  </si>
-  <si>
-    <t>@jasondebolt What is your goal to do with your wealth from #Tsla?</t>
-  </si>
-  <si>
-    <t>@wyldeAF @jasondebolt Same here. A majority of my coworkers as well. There is no second best! #tsla</t>
-  </si>
-  <si>
-    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/98lyq3evGq</t>
-  </si>
-  <si>
-    <t>The Big Five #FAANG Stock and Sector Service is now posted for Wednesday #AMZN #AAPL #FB #NFLX #TSLA #GOOGL and  Sector Funds - #IBB #IYR #XLE #XLE #XLF #XLK #XRT    (link: https://t.co/bihMz399my)   #trading #investing #FinancialFreedom https://t.co/xAPMeXgV44</t>
-  </si>
-  <si>
-    <t>Tesla ⚡️: Starship, 4680 Battery &amp;amp; Positive NHTSA Updates!
-#TheTeslaSpace #TSLA 
-• FAA Pushed Starship to 4/29
-• New 4680 Patten Released
-• Significant Faster Production
-• NHTSA Increase Penalties That will Generate More Regulatory Credits for Tesla 
-https://t.co/9H5nNKHRRK https://t.co/iqvryquOPx</t>
-  </si>
-  <si>
-    <t>Posted Daily Analyses/Updates:
-#SP500 #SPX 
-#VIX $VIX
-#Bitcoin #BTCUSD 
-#TSLA $TSLA
-https://t.co/qLx4srPGAT
-https://t.co/6ISQ7l9Zro
-https://t.co/ZGX5F02AoT
-https://t.co/nU40kNanGt
-https://t.co/5V41NUfCij
-Alerts:
-#gold $GLD
-#silver $SLV
-https://t.co/XHPxshnZuM</t>
-  </si>
-  <si>
-    <t>Heavy #Options Flow &amp;gt; $500K – End of day Fat Prints 
-$TSLA #TSLA 1150C 4-1   --&amp;gt;&amp;gt;  $19 MIL. PRINT
-$AMD #AMD 127C 4-1       --&amp;gt;&amp;gt;  $800k   PRINT
-$DDOG #DDOG 160C 5-20 --&amp;gt;&amp;gt; 7.8 MIL. PRINT
-Game changer Data courtesy of @chatterQuant 
-Source: https://t.co/ug9CyDpSas https://t.co/5fjhyvXgDd</t>
-  </si>
-  <si>
-    <t>What is Twitter talking about ?
-#TSLA #AAPL #MU #AMZN #AMC #FB #QQQ #PYPL
-Source: https://t.co/ug9CyDpSas https://t.co/wPW6txHTCD</t>
-  </si>
-  <si>
-    <t>@hershohm @SawyerMerritt Very real possibility. #TSLA https://t.co/51Q9dLHn57</t>
-  </si>
-  <si>
-    <t>$TSLA - Baglino Andrew D sold 7000.0 shares of Common Stock worth $3,947,020.00 in 2 transaction(s) on 2022-03-28  #TSLA</t>
-  </si>
-  <si>
-    <t>The Market's Beginning To Take MULN STOCK Seriously. 100% gains incoming... https://t.co/7Gf9zj2zgi via @YouTube #muln #MULNSQUEEZE #mulnarmy #mulnapes #stocks #stockmarket #NASDAQ100 #nasdaq #wallstreetbets #WallStreet #tsla #tesla</t>
-  </si>
-  <si>
-    <t>It’s @elonmusk though that gives me anxiety &amp;amp; he’s pretty cute what if I giggle…or mess up &amp;amp; call him dude or bro? God forbid I mention @JeffBezos *trust me I’ve heard stories* anyway @elonmusk I’m pretty sleepy &amp;amp; about to take a nap congrats on a marvelous Q1 #TSLA https://t.co/EZnWvUGpqm</t>
-  </si>
-  <si>
-    <t>#Tesla #Tsla #Teslastock 
-In a stock split the number of outstanding shares increases and the price per share decreases proportionately, while the market capitalization and the value of the company do not change. https://t.co/xIRjp5YpsY</t>
-  </si>
-  <si>
-    <t>My co-worker is now looking and reading more about finance management, trading and investing (stocks and crypto) for a target financial stability when he retires from the Military 💪💪. It feels good to be a positive influence👊. You? how did your day went today? #HYMC #TSLA #CEI</t>
-  </si>
-  <si>
-    <t>Our new car has arrived! #TSLA #zeroemmissions @ Barrie, Ontario https://t.co/rpZ7uYLhdL</t>
-  </si>
-  <si>
-    <t>#Tesla #Tsla #Teslastock 
-     Why Is TESLA Splitting ?
-1.  Share Affordability
-2. Improve Trading Liquidity
-     Why Is Share Affordability
-Important For Tesla As A Company ?
-Just So You Know...
-Company Berkshire Hathaway, which hasn't ever had a stock split in its history.</t>
-  </si>
-  <si>
-    <t>$TSLA working its way into the top 10 most mentioned on wallstreetbets over the last 7 days_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #investors https://t.co/AL16lqrvvd</t>
-  </si>
-  <si>
-    <t>https://t.co/6rXZFDtprv
-Streaming today’s Stock Market recap. Everyone welcome to join and ask questions. 
-#SPY #TSLA $MULN</t>
-  </si>
-  <si>
-    <t>I jumped on #Tsla at the right time.</t>
-  </si>
-  <si>
-    <t>$TSLA seeing an uptick in chatter on wallstreetbets over the last 24 hours_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #investing https://t.co/1OSL323qEa</t>
-  </si>
-  <si>
-    <t>New to Finance Twitter, what account should I follow? #StockMarket #Investing #Finance #SP500 #NASDAQ #TSLA #MSFT #AAPL #FB #AMZN #BA #Crypto #Coinbase</t>
-  </si>
-  <si>
-    <t>LIMITED TIME OFFER: Get 5 FREE stocks valued up to $9,600 by opening &amp;amp; funding a #Webull brokerage account! Get started &amp;gt; #BTC #MMAT #Zilliqa
-#TSLA #YOMTVRaps #HipHop #Verzuz #NFT #Stocks #Stockmarket #NFTCommunity #CarlosEMendez https://t.co/YqRmgEv99k https://t.co/1BAMscYwTA</t>
-  </si>
-  <si>
-    <t>31-03-2022 08:33</t>
-  </si>
-  <si>
-    <t>31-03-2022 08:25</t>
-  </si>
-  <si>
-    <t>31-03-2022 08:10</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:55</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:53</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:45</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:42</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:36</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:29</t>
-  </si>
-  <si>
-    <t>31-03-2022 07:17</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:56</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:48</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:40</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:30</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:25</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:20</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:09</t>
-  </si>
-  <si>
-    <t>31-03-2022 05:05</t>
-  </si>
-  <si>
-    <t>31-03-2022 04:25</t>
-  </si>
-  <si>
-    <t>31-03-2022 04:19</t>
-  </si>
-  <si>
-    <t>31-03-2022 04:15</t>
-  </si>
-  <si>
-    <t>31-03-2022 03:56</t>
-  </si>
-  <si>
-    <t>31-03-2022 02:59</t>
-  </si>
-  <si>
-    <t>31-03-2022 02:47</t>
-  </si>
-  <si>
-    <t>31-03-2022 02:44</t>
-  </si>
-  <si>
-    <t>31-03-2022 02:41</t>
-  </si>
-  <si>
-    <t>31-03-2022 02:28</t>
-  </si>
-  <si>
-    <t>31-03-2022 01:58</t>
-  </si>
-  <si>
-    <t>31-03-2022 01:49</t>
-  </si>
-  <si>
-    <t>31-03-2022 01:23</t>
-  </si>
-  <si>
-    <t>31-03-2022 01:14</t>
-  </si>
-  <si>
-    <t>31-03-2022 01:01</t>
-  </si>
-  <si>
-    <t>31-03-2022 00:24</t>
-  </si>
-  <si>
-    <t>31-03-2022 00:12</t>
-  </si>
-  <si>
-    <t>31-03-2022 00:08</t>
-  </si>
-  <si>
-    <t>30-03-2022 23:19</t>
-  </si>
-  <si>
-    <t>30-03-2022 23:17</t>
-  </si>
-  <si>
-    <t>30-03-2022 22:33</t>
-  </si>
-  <si>
-    <t>30-03-2022 22:32</t>
-  </si>
-  <si>
-    <t>30-03-2022 21:44</t>
-  </si>
-  <si>
-    <t>30-03-2022 21:19</t>
-  </si>
-  <si>
-    <t>30-03-2022 21:14</t>
-  </si>
-  <si>
-    <t>30-03-2022 21:11</t>
-  </si>
-  <si>
-    <t>30-03-2022 21:08</t>
-  </si>
-  <si>
-    <t>30-03-2022 20:58</t>
-  </si>
-  <si>
-    <t>30-03-2022 20:50</t>
-  </si>
-  <si>
-    <t>30-03-2022 20:47</t>
-  </si>
-  <si>
-    <t>30-03-2022 20:40</t>
-  </si>
-  <si>
-    <t>30-03-2022 20:28</t>
-  </si>
-  <si>
-    <t>13-11-2021 19:14</t>
-  </si>
-  <si>
-    <t>25-02-2010 05:59</t>
-  </si>
-  <si>
-    <t>04-08-2017 02:58</t>
-  </si>
-  <si>
-    <t>08-04-2021 09:31</t>
-  </si>
-  <si>
-    <t>28-11-2020 04:42</t>
+$TSLA #Tesla #TSLA #TeslaStock #ElonMusk #SenatorKaren https://t.co/2Ah7lBRlXl</t>
+  </si>
+  <si>
+    <t>#TSLA My track record shows I know when to short Tesla ..! https://t.co/HaiXfMhyJp</t>
+  </si>
+  <si>
+    <t>$TSLA HP bounce zone at confluence of flag bottom and support around 1070 .
+Also can reject at 1090 .
+Calls above 1090 if it breaks with PT at 1100.
+#TSLA #Tesla #ElonMusk #ChartoftheDay #options #ElectricVehicles https://t.co/HUoyLIGU79</t>
+  </si>
+  <si>
+    <t>$TSLA 👀 Forming a bull flag after it rejected off 1115- 1120 zone. 
+If 1070 breaks, then PTs are 1055 and 1040 for sure.
+#Tesla #ElonMusk #TSLA #Tradeidea #optionstrade #ElectricVehicles #Bullish https://t.co/WXULCfUr2U</t>
+  </si>
+  <si>
+    <t>@teslaownersSV @elonmusk Me tomorrow morning after I tell work I’m sick…Sick of working there cause 🩳  ARE GONNA EAT CROW!! #MOASS #GME #AMC #TSLA #HYMC</t>
+  </si>
+  <si>
+    <t>@VoltBossBaby @ShibaArchives $Volt is going to be parabolic soon #VOLT #VOLTINU #VOLTARMY #ETH #BNB #TSLA @VoltInuOfficial @VoltArmy_ @cz_binance @ChinaPumpCN @elonmusk @VitalikButerin @pablo_cro @TheGen35 @icryptocare @LuckyTruong75 https://t.co/EEPqaR80NK</t>
+  </si>
+  <si>
+    <t>Domain Name For Sale
+https://t.co/efsHn3CsYl
+.
+#Domains #domainnameforsale #domainsforsale #cryptocurrency #Coinbase  #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3Coin #DAO https://t.co/9cfNugucOk</t>
+  </si>
+  <si>
+    <t>$TSLA $NIO $XPEV $LI.. all eyes on supply chain/production as EV makers prepare to release quarterly deliveries..
+https://t.co/4qz8rp7FzP
+#tsla #teslastock #tesla #nio #niostock #marchquarterdeliveries</t>
+  </si>
+  <si>
+    <t>@Tesla #TSLA short. This technology is insane and unsustainable. Besides what if you have a disagreement with the owner. He can shut your car down! https://t.co/nQR34bA1Jh</t>
+  </si>
+  <si>
+    <t>FREE WATCHLIST WIH ENTRY PRICE AND PRICE TARGETS 
+#tsla #twtr #snap #snow $snow $tsa $snap 
+$twtr #gme #amc $gme $amc https://t.co/YpJ1Zm45dq</t>
+  </si>
+  <si>
+    <t>#tesla #tsla Tesla $1150 Monday after q1 deliveries on the weekend, tesla $1250 all time high Friday with Texas party opening. Possible?</t>
+  </si>
+  <si>
+    <t>$TSLA gappy-gap-gap
+#optionflow #StockMarket #OptionsTrading #options #wallstreet #Daytrade #stocks #tsla https://t.co/DQ0Du3LQWX</t>
+  </si>
+  <si>
+    <t>#TSLA puts?? 🧐 https://t.co/VaEPrXiL8A</t>
+  </si>
+  <si>
+    <t>@srj5679 @jimcramer If Cramer says it gonna tank, better go all-in. That’s what Ive learned. #TSLA</t>
+  </si>
+  <si>
+    <t>Domain Name For Sale
+https://t.co/EOQhFILek7
+.
+#Domains #domainnameforsale #domainsforsale #cryptocurrency #cryptotrading #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3Coin https://t.co/ibXs7a4rcM</t>
+  </si>
+  <si>
+    <t>Domain Name For Sale
+https://t.co/gsVU2vOJcc
+.
+#Domains #domainnameforsale #domainsforsale #cryptocurrency #cryptotrading #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3 #Wallet https://t.co/URx52bOp2n</t>
+  </si>
+  <si>
+    <t>$tsla #TSLA | D | Hit 2nd ring #geocharting #marketgeometry #nextgentools #gocharting https://t.co/XvnHPlSAen</t>
+  </si>
+  <si>
+    <t>@cbcmarketplace Interesting… just wondering, can a #tesla be stolen in the same fashion, too? No key holes, no push start button. #ElectricVehicles #TSLA @tesla @elonmusk https://t.co/FM8vx6VYEp</t>
+  </si>
+  <si>
+    <t>@matthew35746729 @Jefferies @Yahoo Absolutely Matthew!  #Tesla #Brother!  
+#TSLA @Tesla</t>
+  </si>
+  <si>
+    <t>$TSLA #TSLA no change here as IMO retrace should continue lower.
+R1 pivot $1065.20 and pwHighs $1040.70 to be tested with a gap to fill much lower. 
+Call volume has been outflowing. Waiting to see Put volume increase. 
+#stocks https://t.co/zw6Td9e5CI https://t.co/jf2qln7QPT</t>
+  </si>
+  <si>
+    <t>Report: Tesla Giga Shanghai Will Extend Plant Suspension #TSLA #ElonMusk #Tesla #Sustainability #SDGs [Video]: The Tesla Giga Shanghai plant has suspended production of electric cars for several days, but it might not be the end of COVID-19-related… https://t.co/MHDoOaKq5H https://t.co/QQ2CL496IH</t>
+  </si>
+  <si>
+    <t>Report: Tesla Giga Shanghai Will Extend Plant Suspension #TSLA #ElonMusk #Tesla #Sustainability #SDGs [Video]: The Tesla Giga Shanghai plant has suspended production of electric cars for several days, but it might not be the end of COVID-19-related… https://t.co/ZOHltlE5QL https://t.co/ILc6mUVeE5</t>
+  </si>
+  <si>
+    <t>Why do people sell their stocks?
+Cause they need money to buy the stocks at a higher price lol 🤣🤣🤣
+#Truestory $TSLA #TSLA</t>
+  </si>
+  <si>
+    <t>TESLA-SELL strategy - #TSLA chart on @TradingView https://t.co/mkyoAoFqqY</t>
+  </si>
+  <si>
+    <t>#TSLA going to 1095 in 5 days? Hopefully. https://t.co/bLeA9kSpUt</t>
+  </si>
+  <si>
+    <t>We are hosting our daily market charting workshop on Discord.
+In these workshop:
+1. We do technical analysis 📈
+2. Plan our trades for coming days ✍️
+3. Q&amp;amp;A with our members 🗣️
+Try it for yourself with a 3-day Risk free trial:
+https://t.co/EpGQOYlg7k
+#WallStreet #tsla #SPX #SPY https://t.co/6mdof3FAJ3</t>
+  </si>
+  <si>
+    <t>The price of a commodity will never go to zero. When you invest in commodities futures, you are not buying a piece of paper that says you own an intangible of the company that can go bankrupt. #AMZN #tsla #TradingView https://t.co/xzxrra8FRp</t>
+  </si>
+  <si>
+    <t>@GrunzkeLukas @DoctorJack16 The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@DoctorJack16 #NIO not because they will overtake #TSLA per se, but with a 30 billion dollar market cap with a good chance to be the market leader in China (soon to be largest economy in the world), the upside is far greater imo</t>
+  </si>
+  <si>
+    <t>Serviced my 22 Model 3 for a rattle/squeak. Service was great, fast, got it done. @Tesla #tsla</t>
+  </si>
+  <si>
+    <t>01-04-2022 09:23</t>
+  </si>
+  <si>
+    <t>01-04-2022 09:16</t>
+  </si>
+  <si>
+    <t>01-04-2022 09:02</t>
+  </si>
+  <si>
+    <t>01-04-2022 08:22</t>
+  </si>
+  <si>
+    <t>01-04-2022 08:20</t>
+  </si>
+  <si>
+    <t>01-04-2022 08:19</t>
+  </si>
+  <si>
+    <t>01-04-2022 08:02</t>
+  </si>
+  <si>
+    <t>01-04-2022 07:57</t>
+  </si>
+  <si>
+    <t>01-04-2022 07:35</t>
+  </si>
+  <si>
+    <t>01-04-2022 07:29</t>
+  </si>
+  <si>
+    <t>01-04-2022 07:02</t>
+  </si>
+  <si>
+    <t>01-04-2022 06:17</t>
+  </si>
+  <si>
+    <t>01-04-2022 06:10</t>
+  </si>
+  <si>
+    <t>01-04-2022 05:54</t>
+  </si>
+  <si>
+    <t>01-04-2022 05:52</t>
+  </si>
+  <si>
+    <t>01-04-2022 05:51</t>
+  </si>
+  <si>
+    <t>01-04-2022 05:50</t>
+  </si>
+  <si>
+    <t>01-04-2022 05:30</t>
+  </si>
+  <si>
+    <t>01-04-2022 05:28</t>
+  </si>
+  <si>
+    <t>01-04-2022 04:52</t>
+  </si>
+  <si>
+    <t>01-04-2022 04:47</t>
+  </si>
+  <si>
+    <t>01-04-2022 04:46</t>
+  </si>
+  <si>
+    <t>01-04-2022 04:28</t>
+  </si>
+  <si>
+    <t>01-04-2022 04:00</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:59</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:37</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:29</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:25</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:24</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:19</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:18</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:15</t>
+  </si>
+  <si>
+    <t>01-04-2022 03:00</t>
+  </si>
+  <si>
+    <t>01-04-2022 02:33</t>
+  </si>
+  <si>
+    <t>01-04-2022 02:22</t>
+  </si>
+  <si>
+    <t>01-04-2022 02:17</t>
+  </si>
+  <si>
+    <t>01-04-2022 02:09</t>
+  </si>
+  <si>
+    <t>01-04-2022 01:18</t>
+  </si>
+  <si>
+    <t>01-04-2022 01:01</t>
+  </si>
+  <si>
+    <t>01-04-2022 00:42</t>
+  </si>
+  <si>
+    <t>01-04-2022 00:38</t>
+  </si>
+  <si>
+    <t>01-04-2022 00:24</t>
+  </si>
+  <si>
+    <t>01-04-2022 00:19</t>
+  </si>
+  <si>
+    <t>01-04-2022 00:00</t>
+  </si>
+  <si>
+    <t>20-05-2018 10:40</t>
+  </si>
+  <si>
+    <t>13-09-2021 11:07</t>
+  </si>
+  <si>
+    <t>11-01-2021 09:26</t>
+  </si>
+  <si>
+    <t>27-12-2018 21:52</t>
+  </si>
+  <si>
+    <t>29-06-2011 20:11</t>
+  </si>
+  <si>
+    <t>03-02-2009 10:18</t>
+  </si>
+  <si>
+    <t>14-01-2020 01:27</t>
+  </si>
+  <si>
+    <t>03-01-2011 23:47</t>
+  </si>
+  <si>
+    <t>27-01-2019 23:03</t>
   </si>
   <si>
     <t>30-08-2011 12:26</t>
   </si>
   <si>
-    <t>30-09-2017 19:06</t>
-  </si>
-  <si>
-    <t>31-10-2015 10:02</t>
+    <t>20-07-2020 10:59</t>
   </si>
   <si>
     <t>08-01-2020 17:10</t>
   </si>
   <si>
-    <t>22-03-2022 20:47</t>
-  </si>
-  <si>
-    <t>07-01-2022 06:16</t>
+    <t>06-12-2010 23:58</t>
   </si>
   <si>
     <t>14-04-2009 23:28</t>
   </si>
   <si>
-    <t>17-12-2021 04:44</t>
-  </si>
-  <si>
-    <t>17-03-2021 13:22</t>
-  </si>
-  <si>
-    <t>29-05-2014 05:06</t>
-  </si>
-  <si>
-    <t>13-10-2021 02:40</t>
-  </si>
-  <si>
-    <t>13-02-2017 20:51</t>
-  </si>
-  <si>
-    <t>19-07-2017 19:21</t>
+    <t>21-10-2020 22:09</t>
+  </si>
+  <si>
+    <t>31-03-2022 02:51</t>
+  </si>
+  <si>
+    <t>02-03-2011 00:30</t>
+  </si>
+  <si>
+    <t>28-01-2022 23:19</t>
+  </si>
+  <si>
+    <t>08-02-2022 20:08</t>
+  </si>
+  <si>
+    <t>26-09-2016 18:29</t>
+  </si>
+  <si>
+    <t>01-03-2022 04:23</t>
+  </si>
+  <si>
+    <t>25-06-2010 17:56</t>
+  </si>
+  <si>
+    <t>03-11-2009 16:30</t>
+  </si>
+  <si>
+    <t>05-03-2017 02:14</t>
+  </si>
+  <si>
+    <t>09-01-2018 05:26</t>
+  </si>
+  <si>
+    <t>30-09-2014 21:51</t>
+  </si>
+  <si>
+    <t>08-07-2019 00:06</t>
+  </si>
+  <si>
+    <t>15-08-2021 22:14</t>
+  </si>
+  <si>
+    <t>21-11-2020 19:42</t>
   </si>
   <si>
     <t>10-12-2016 04:42</t>
   </si>
   <si>
-    <t>22-06-2020 00:03</t>
-  </si>
-  <si>
-    <t>24-10-2020 11:31</t>
-  </si>
-  <si>
-    <t>01-09-2011 09:24</t>
-  </si>
-  <si>
-    <t>24-04-2021 05:45</t>
-  </si>
-  <si>
-    <t>19-01-2017 03:39</t>
-  </si>
-  <si>
-    <t>09-07-2021 16:16</t>
-  </si>
-  <si>
-    <t>23-11-2021 02:22</t>
-  </si>
-  <si>
-    <t>18-01-2017 02:58</t>
-  </si>
-  <si>
-    <t>28-09-2021 20:44</t>
-  </si>
-  <si>
-    <t>25-08-2020 16:39</t>
-  </si>
-  <si>
-    <t>28-05-2020 02:39</t>
-  </si>
-  <si>
-    <t>30-12-2019 01:46</t>
-  </si>
-  <si>
-    <t>25-10-2020 07:23</t>
-  </si>
-  <si>
-    <t>31-05-2010 16:38</t>
-  </si>
-  <si>
-    <t>30-03-2022 17:05</t>
-  </si>
-  <si>
-    <t>29-01-2013 11:00</t>
-  </si>
-  <si>
-    <t>[{'text': 'ElonMusk', 'indices': [76, 85]}, {'text': 'Tesla', 'indices': [86, 92]}, {'text': 'Musk', 'indices': [93, 98]}, {'text': 'TSLA', 'indices': [99, 104]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'btc', 'indices': [25, 29]}, {'text': 'tsla', 'indices': [58, 63]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'eth', 'indices': [74, 78]}, {'text': 'tsla', 'indices': [79, 84]}, {'text': 'shib', 'indices': [85, 90]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tesla', 'indices': [26, 32]}, {'text': 'tsla', 'indices': [33, 38]}, {'text': 'stock', 'indices': [39, 45]}, {'text': 'stockmarket', 'indices': [46, 58]}, {'text': 'options', 'indices': [59, 67]}, {'text': 'money', 'indices': [68, 74]}, {'text': 'cars', 'indices': [75, 80]}, {'text': 'tech', 'indices': [81, 86]}, {'text': 'technology', 'indices': [87, 98]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [40, 45]}, {'text': 'BDY', 'indices': [46, 50]}, {'text': 'NIO', 'indices': [51, 55]}, {'text': 'V2L', 'indices': [56, 60]}, {'text': 'EVCHARGER', 'indices': [61, 71]}, {'text': 'HYUNDAI', 'indices': [72, 80]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [34, 39]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [29, 34]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [13, 18]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Uphold', 'indices': [37, 44]}, {'text': 'btc', 'indices': [63, 67]}, {'text': 'eth', 'indices': [68, 72]}, {'text': 'tsla', 'indices': [83, 88]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Uphold', 'indices': [35, 42]}, {'text': 'btc', 'indices': [61, 65]}, {'text': 'eth', 'indices': [66, 70]}, {'text': 'tsla', 'indices': [81, 86]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'shitadel', 'indices': [133, 142]}, {'text': 'susqueshit', 'indices': [144, 155]}, {'text': 'simpleshit', 'indices': [157, 168]}, {'text': 'change', 'indices': [192, 199]}, {'text': 'TSLA', 'indices': [230, 235]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [102, 107]}, {'text': 'wallstreetbets', 'indices': [111, 126]}, {'text': 'trading', 'indices': [128, 136]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [17, 22]}, {'text': 'OptionsTrading', 'indices': [23, 38]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'SPY', 'indices': [167, 171]}, {'text': 'TSLA', 'indices': [172, 177]}, {'text': 'markets', 'indices': [179, 187]}, {'text': 'DayTrading', 'indices': [188, 199]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [90, 96]}, {'text': 'TSLA', 'indices': [97, 102]}, {'text': 'TeslaStock', 'indices': [103, 114]}, {'text': 'ElonMusk', 'indices': [115, 124]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [40, 45]}]</t>
+    <t>08-09-2008 22:56</t>
+  </si>
+  <si>
+    <t>07-05-2020 18:13</t>
+  </si>
+  <si>
+    <t>08-04-2018 16:19</t>
+  </si>
+  <si>
+    <t>18-09-2010 07:23</t>
+  </si>
+  <si>
+    <t>18-03-2022 00:09</t>
+  </si>
+  <si>
+    <t>09-12-2013 22:25</t>
+  </si>
+  <si>
+    <t>04-11-2020 09:43</t>
+  </si>
+  <si>
+    <t>07-10-2016 06:39</t>
+  </si>
+  <si>
+    <t>09-08-2016 20:38</t>
+  </si>
+  <si>
+    <t>[{'text': 'newmonth', 'indices': [59, 68]}, {'text': 'bitcoin', 'indices': [69, 77]}, {'text': 'ethereum', 'indices': [78, 87]}, {'text': 'btc', 'indices': [88, 92]}, {'text': 'satoshi', 'indices': [93, 101]}, {'text': 'cryptonews', 'indices': [102, 113]}, {'text': 'binance', 'indices': [114, 122]}, {'text': 'satoshinakamoto', 'indices': [123, 139]}, {'text': 'btcmemes', 'indices': [140, 149]}, {'text': 'tsla', 'indices': [150, 155]}, {'text': 'wallstreetbets', 'indices': [156, 171]}, {'text': 'metaverse', 'indices': [172, 182]}, {'text': 'defi', 'indices': [183, 188]}, {'text': 'nft', 'indices': [189, 193]}, {'text': 'dogecoin', 'indices': [194, 203]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tesla', 'indices': [29, 35]}, {'text': 'tsla', 'indices': [36, 41]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Shortsqueeze', 'indices': [46, 59]}, {'text': 'LegalizeWeed', 'indices': [60, 73]}, {'text': 'Cannabis', 'indices': [74, 83]}, {'text': 'Wallstreetbets', 'indices': [84, 99]}, {'text': 'Reddit', 'indices': [101, 108]}, {'text': 'Stonks', 'indices': [109, 116]}, {'text': 'GME', 'indices': [117, 121]}, {'text': 'AMC', 'indices': [122, 126]}, {'text': 'TSLA', 'indices': [127, 132]}, {'text': 'Elondoge', 'indices': [133, 142]}, {'text': 'Bitcoin', 'indices': [143, 151]}, {'text': 'Apes', 'indices': [152, 157]}, {'text': 'Shib', 'indices': [158, 163]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'pltr', 'indices': [30, 35]}, {'text': 'tsla', 'indices': [64, 69]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [48, 53]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [23, 28]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'GME', 'indices': [101, 105]}, {'text': 'AMC', 'indices': [106, 110]}, {'text': 'SNDL', 'indices': [112, 117]}, {'text': 'TSLA', 'indices': [119, 124]}, {'text': 'WISH', 'indices': [126, 131]}, {'text': 'JMIA', 'indices': [132, 137]}, {'text': 'BIGC', 'indices': [138, 143]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [7, 12]}, {'text': 'Tesla', 'indices': [54, 60]}]</t>
   </si>
   <si>
     <t>[{'text': 'TSLA', 'indices': [6, 11]}]</t>
   </si>
   <si>
-    <t>[{'text': 'CyberRodeo', 'indices': [53, 64]}, {'text': 'elonamusk', 'indices': [65, 75]}, {'text': 'texasgigafactory', 'indices': [76, 93]}, {'text': 'Tesla', 'indices': [94, 100]}, {'text': 'TSLA', 'indices': [101, 106]}, {'text': 'SpaceX', 'indices': [107, 114]}, {'text': 'Tesla', 'indices': [115, 121]}, {'text': 'Elon', 'indices': [122, 127]}, {'text': 'FSDBeta', 'indices': [128, 136]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [89, 95]}, {'text': 'ElonMusk', 'indices': [96, 105]}, {'text': 'TSLA', 'indices': [106, 111]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [83, 88]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'stocks', 'indices': [272, 279]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tsla', 'indices': [59, 64]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [94, 99]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'FAANG', 'indices': [13, 19]}, {'text': 'AMZN', 'indices': [73, 78]}, {'text': 'AAPL', 'indices': [79, 84]}, {'text': 'FB', 'indices': [85, 88]}, {'text': 'NFLX', 'indices': [89, 94]}, {'text': 'TSLA', 'indices': [95, 100]}, {'text': 'GOOGL', 'indices': [101, 107]}, {'text': 'IBB', 'indices': [128, 132]}, {'text': 'IYR', 'indices': [133, 137]}, {'text': 'XLE', 'indices': [138, 142]}, {'text': 'XLE', 'indices': [143, 147]}, {'text': 'XLF', 'indices': [148, 152]}, {'text': 'XLK', 'indices': [153, 157]}, {'text': 'XRT', 'indices': [158, 162]}, {'text': 'trading', 'indices': [200, 208]}, {'text': 'investing', 'indices': [209, 219]}, {'text': 'FinancialFreedom', 'indices': [220, 237]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TheTeslaSpace', 'indices': [63, 77]}, {'text': 'TSLA', 'indices': [78, 83]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'SP500', 'indices': [31, 37]}, {'text': 'SPX', 'indices': [38, 42]}, {'text': 'VIX', 'indices': [44, 48]}, {'text': 'Bitcoin', 'indices': [54, 62]}, {'text': 'BTCUSD', 'indices': [63, 70]}, {'text': 'TSLA', 'indices': [72, 77]}, {'text': 'gold', 'indices': [214, 219]}, {'text': 'silver', 'indices': [225, 232]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Options', 'indices': [6, 14]}, {'text': 'TSLA', 'indices': [64, 69]}, {'text': 'AMD', 'indices': [115, 119]}, {'text': 'DDOG', 'indices': [168, 173]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [33, 38]}, {'text': 'AAPL', 'indices': [39, 44]}, {'text': 'MU', 'indices': [45, 48]}, {'text': 'AMZN', 'indices': [49, 54]}, {'text': 'AMC', 'indices': [55, 59]}, {'text': 'FB', 'indices': [60, 63]}, {'text': 'QQQ', 'indices': [64, 68]}, {'text': 'PYPL', 'indices': [69, 74]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [48, 53]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [115, 120]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'muln', 'indices': [113, 118]}, {'text': 'MULNSQUEEZE', 'indices': [119, 131]}, {'text': 'mulnarmy', 'indices': [132, 141]}, {'text': 'mulnapes', 'indices': [142, 151]}, {'text': 'stocks', 'indices': [152, 159]}, {'text': 'stockmarket', 'indices': [160, 172]}, {'text': 'NASDAQ100', 'indices': [173, 183]}, {'text': 'nasdaq', 'indices': [184, 191]}, {'text': 'wallstreetbets', 'indices': [192, 207]}, {'text': 'WallStreet', 'indices': [208, 219]}, {'text': 'tsla', 'indices': [220, 225]}, {'text': 'tesla', 'indices': [226, 232]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [273, 278]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [0, 6]}, {'text': 'Tsla', 'indices': [7, 12]}, {'text': 'Teslastock', 'indices': [13, 24]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'HYMC', 'indices': [261, 266]}, {'text': 'TSLA', 'indices': [267, 272]}, {'text': 'CEI', 'indices': [273, 277]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [25, 30]}, {'text': 'zeroemmissions', 'indices': [31, 46]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [122, 127]}, {'text': 'wallstreetbets', 'indices': [131, 146]}, {'text': 'investors', 'indices': [148, 158]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'SPY', 'indices': [109, 113]}, {'text': 'TSLA', 'indices': [114, 119]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tsla', 'indices': [12, 17]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [105, 110]}, {'text': 'wallstreetbets', 'indices': [114, 129]}, {'text': 'investing', 'indices': [131, 141]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'StockMarket', 'indices': [54, 66]}, {'text': 'Investing', 'indices': [67, 77]}, {'text': 'Finance', 'indices': [78, 86]}, {'text': 'SP500', 'indices': [87, 93]}, {'text': 'NASDAQ', 'indices': [94, 101]}, {'text': 'TSLA', 'indices': [102, 107]}, {'text': 'MSFT', 'indices': [108, 113]}, {'text': 'AAPL', 'indices': [114, 119]}, {'text': 'FB', 'indices': [120, 123]}, {'text': 'AMZN', 'indices': [124, 129]}, {'text': 'BA', 'indices': [130, 133]}, {'text': 'Crypto', 'indices': [134, 141]}, {'text': 'Coinbase', 'indices': [142, 151]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Webull', 'indices': [85, 92]}, {'text': 'BTC', 'indices': [129, 133]}, {'text': 'MMAT', 'indices': [134, 139]}, {'text': 'Zilliqa', 'indices': [140, 148]}, {'text': 'TSLA', 'indices': [149, 154]}, {'text': 'YOMTVRaps', 'indices': [155, 165]}, {'text': 'HipHop', 'indices': [166, 173]}, {'text': 'Verzuz', 'indices': [174, 181]}, {'text': 'NFT', 'indices': [182, 186]}, {'text': 'Stocks', 'indices': [187, 194]}, {'text': 'Stockmarket', 'indices': [195, 207]}, {'text': 'NFTCommunity', 'indices': [208, 221]}, {'text': 'CarlosEMendez', 'indices': [222, 236]}]</t>
+    <t>[{'text': 'tsla', 'indices': [10, 15]}, {'text': 'StocksToBuy', 'indices': [22, 34]}, {'text': 'StockSplit', 'indices': [36, 47]}, {'text': 'stockstowatch', 'indices': [49, 63]}, {'text': 'bullsarein', 'indices': [64, 75]}, {'text': 'WHALES', 'indices': [76, 83]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'SPACEX', 'indices': [118, 125]}, {'text': 'Tesla', 'indices': [127, 133]}, {'text': 'TSLA', 'indices': [135, 140]}, {'text': 'TSLAQ', 'indices': [142, 148]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [124, 129]}, {'text': 'wallstreetbets', 'indices': [133, 148]}, {'text': 'stockmarket', 'indices': [150, 162]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [32, 37]}, {'text': 'stock', 'indices': [49, 55]}, {'text': 'shareholders', 'indices': [56, 69]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'StockMarket', 'indices': [4, 16]}, {'text': 'tsla', 'indices': [46, 51]}, {'text': 'tsla', 'indices': [99, 104]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [123, 128]}, {'text': 'ElonMusk', 'indices': [129, 138]}, {'text': 'Monkeys', 'indices': [140, 148]}, {'text': 'TSLA', 'indices': [150, 155]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [90, 95]}, {'text': 'ElonMusk', 'indices': [96, 105]}, {'text': 'Monkeys', 'indices': [107, 115]}, {'text': 'TSLA', 'indices': [117, 122]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [88, 93]}, {'text': 'ElonMusk', 'indices': [94, 103]}, {'text': 'Monkeys', 'indices': [105, 113]}, {'text': 'TSLA', 'indices': [115, 120]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [79, 84]}, {'text': 'ElonMusk', 'indices': [85, 94]}, {'text': 'Monkeys', 'indices': [96, 104]}, {'text': 'TSLA', 'indices': [106, 111]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [83, 88]}, {'text': 'ElonMusk', 'indices': [89, 98]}, {'text': 'Monkeys', 'indices': [100, 108]}, {'text': 'TSLA', 'indices': [110, 115]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [80, 85]}, {'text': 'ElonMusk', 'indices': [86, 95]}, {'text': 'Monkeys', 'indices': [97, 105]}, {'text': 'TSLA', 'indices': [107, 112]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [96, 102]}, {'text': 'TSLA', 'indices': [103, 108]}, {'text': 'TeslaStock', 'indices': [109, 120]}, {'text': 'ElonMusk', 'indices': [121, 130]}, {'text': 'SenatorKaren', 'indices': [131, 144]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [0, 5]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [149, 154]}, {'text': 'Tesla', 'indices': [155, 161]}, {'text': 'ElonMusk', 'indices': [162, 171]}, {'text': 'ChartoftheDay', 'indices': [172, 186]}, {'text': 'options', 'indices': [187, 195]}, {'text': 'ElectricVehicles', 'indices': [196, 213]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [121, 127]}, {'text': 'ElonMusk', 'indices': [128, 137]}, {'text': 'TSLA', 'indices': [138, 143]}, {'text': 'Tradeidea', 'indices': [144, 154]}, {'text': 'optionstrade', 'indices': [155, 168]}, {'text': 'ElectricVehicles', 'indices': [169, 186]}, {'text': 'Bullish', 'indices': [187, 195]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'MOASS', 'indices': [124, 130]}, {'text': 'GME', 'indices': [131, 135]}, {'text': 'AMC', 'indices': [136, 140]}, {'text': 'TSLA', 'indices': [141, 146]}, {'text': 'HYMC', 'indices': [147, 152]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'VOLT', 'indices': [65, 70]}, {'text': 'VOLTINU', 'indices': [71, 79]}, {'text': 'VOLTARMY', 'indices': [80, 89]}, {'text': 'ETH', 'indices': [90, 94]}, {'text': 'BNB', 'indices': [95, 99]}, {'text': 'TSLA', 'indices': [100, 105]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'Coinbase', 'indices': [107, 116]}, {'text': 'Crypto', 'indices': [118, 125]}, {'text': 'Cryptos', 'indices': [126, 134]}, {'text': 'cryptogiveaway', 'indices': [135, 150]}, {'text': 'CryptocurrencyNews', 'indices': [151, 170]}, {'text': 'Bitcoin', 'indices': [171, 179]}, {'text': 'cryptobank', 'indices': [180, 191]}, {'text': 'cryptowallet', 'indices': [192, 205]}, {'text': 'BTC', 'indices': [206, 210]}, {'text': 'Ethereum', 'indices': [211, 220]}, {'text': 'ETH', 'indices': [221, 225]}, {'text': 'tezos', 'indices': [226, 232]}, {'text': 'doge', 'indices': [233, 238]}, {'text': 'TSLA', 'indices': [239, 244]}, {'text': 'NFT', 'indices': [245, 249]}, {'text': 'blockchain', 'indices': [250, 261]}, {'text': 'Web3Coin', 'indices': [262, 271]}, {'text': 'DAO', 'indices': [272, 276]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [140, 145]}, {'text': 'teslastock', 'indices': [146, 157]}, {'text': 'tesla', 'indices': [158, 164]}, {'text': 'nio', 'indices': [165, 169]}, {'text': 'niostock', 'indices': [170, 179]}, {'text': 'marchquarterdeliveries', 'indices': [180, 203]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [7, 12]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [50, 55]}, {'text': 'twtr', 'indices': [56, 61]}, {'text': 'snap', 'indices': [62, 67]}, {'text': 'snow', 'indices': [68, 73]}, {'text': 'gme', 'indices': [98, 102]}, {'text': 'amc', 'indices': [103, 107]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tesla', 'indices': [0, 6]}, {'text': 'tsla', 'indices': [7, 12]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'optionflow', 'indices': [21, 32]}, {'text': 'StockMarket', 'indices': [33, 45]}, {'text': 'OptionsTrading', 'indices': [46, 61]}, {'text': 'options', 'indices': [62, 70]}, {'text': 'wallstreet', 'indices': [71, 82]}, {'text': 'Daytrade', 'indices': [83, 92]}, {'text': 'stocks', 'indices': [93, 100]}, {'text': 'tsla', 'indices': [101, 106]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [93, 98]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'cryptotrading', 'indices': [107, 121]}, {'text': 'Crypto', 'indices': [122, 129]}, {'text': 'Cryptos', 'indices': [130, 138]}, {'text': 'cryptogiveaway', 'indices': [139, 154]}, {'text': 'CryptocurrencyNews', 'indices': [155, 174]}, {'text': 'Bitcoin', 'indices': [175, 183]}, {'text': 'cryptobank', 'indices': [184, 195]}, {'text': 'cryptowallet', 'indices': [196, 209]}, {'text': 'BTC', 'indices': [210, 214]}, {'text': 'Ethereum', 'indices': [215, 224]}, {'text': 'ETH', 'indices': [225, 229]}, {'text': 'tezos', 'indices': [230, 236]}, {'text': 'doge', 'indices': [237, 242]}, {'text': 'TSLA', 'indices': [243, 248]}, {'text': 'NFT', 'indices': [249, 253]}, {'text': 'blockchain', 'indices': [254, 265]}, {'text': 'Web3Coin', 'indices': [266, 275]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'cryptotrading', 'indices': [107, 121]}, {'text': 'Crypto', 'indices': [122, 129]}, {'text': 'Cryptos', 'indices': [130, 138]}, {'text': 'cryptogiveaway', 'indices': [139, 154]}, {'text': 'CryptocurrencyNews', 'indices': [155, 174]}, {'text': 'Bitcoin', 'indices': [175, 183]}, {'text': 'cryptobank', 'indices': [184, 195]}, {'text': 'cryptowallet', 'indices': [196, 209]}, {'text': 'BTC', 'indices': [210, 214]}, {'text': 'Ethereum', 'indices': [215, 224]}, {'text': 'ETH', 'indices': [225, 229]}, {'text': 'tezos', 'indices': [230, 236]}, {'text': 'doge', 'indices': [237, 242]}, {'text': 'TSLA', 'indices': [243, 248]}, {'text': 'NFT', 'indices': [249, 253]}, {'text': 'blockchain', 'indices': [254, 265]}, {'text': 'Web3', 'indices': [266, 271]}, {'text': 'Wallet', 'indices': [272, 279]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'geocharting', 'indices': [31, 43]}, {'text': 'marketgeometry', 'indices': [44, 59]}, {'text': 'nextgentools', 'indices': [60, 73]}, {'text': 'gocharting', 'indices': [74, 85]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tesla', 'indices': [51, 57]}, {'text': 'ElectricVehicles', 'indices': [130, 147]}, {'text': 'TSLA', 'indices': [148, 153]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [56, 62]}, {'text': 'Brother', 'indices': [63, 71]}, {'text': 'TSLA', 'indices': [76, 81]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'stocks', 'indices': [222, 229]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [57, 62]}, {'text': 'ElonMusk', 'indices': [63, 72]}, {'text': 'Tesla', 'indices': [73, 79]}, {'text': 'Sustainability', 'indices': [80, 95]}, {'text': 'SDGs', 'indices': [96, 101]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Truestory', 'indices': [101, 111]}, {'text': 'TSLA', 'indices': [118, 123]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [22, 27]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'WallStreet', 'indices': [255, 266]}, {'text': 'tsla', 'indices': [267, 272]}, {'text': 'SPX', 'indices': [273, 277]}, {'text': 'SPY', 'indices': [278, 282]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'AMZN', 'indices': [193, 198]}, {'text': 'tsla', 'indices': [199, 204]}, {'text': 'TradingView', 'indices': [205, 217]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [95, 100]}, {'text': 'ElonMusk', 'indices': [101, 110]}, {'text': 'Monkeys', 'indices': [112, 120]}, {'text': 'TSLA', 'indices': [122, 127]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'NIO', 'indices': [14, 18]}, {'text': 'TSLA', 'indices': [50, 55]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [89, 94]}]</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>8514</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1053,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1067,7 +1054,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1064</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
@@ -1079,10 +1066,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1093,22 +1080,22 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1064</v>
+        <v>460</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1119,7 +1106,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1064</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -1131,10 +1118,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1145,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -1157,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
         <v>144</v>
@@ -1171,7 +1158,7 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>1064</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>62</v>
@@ -1183,10 +1170,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1197,7 +1184,7 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -1209,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1223,7 +1210,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>748</v>
+        <v>329</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -1235,10 +1222,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1249,7 +1236,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>1064</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>65</v>
@@ -1261,10 +1248,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1287,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1301,7 +1288,7 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>685</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>67</v>
@@ -1313,10 +1300,10 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1327,7 +1314,7 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>685</v>
+        <v>3140</v>
       </c>
       <c r="D13" t="s">
         <v>68</v>
@@ -1342,7 +1329,7 @@
         <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1353,7 +1340,7 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>1064</v>
+        <v>149</v>
       </c>
       <c r="D14" t="s">
         <v>69</v>
@@ -1365,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H14" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1379,22 +1366,22 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>1064</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H15" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1405,7 +1392,7 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>1064</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
         <v>71</v>
@@ -1417,10 +1404,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1431,13 +1418,13 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>677</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
         <v>72</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1446,7 +1433,7 @@
         <v>113</v>
       </c>
       <c r="H17" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1457,22 +1444,22 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>3141</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1483,10 +1470,10 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>1064</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1495,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1509,10 +1496,10 @@
         <v>25</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1521,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H20" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1535,10 +1522,10 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1547,10 +1534,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H21" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1561,22 +1548,22 @@
         <v>27</v>
       </c>
       <c r="C22">
-        <v>99654</v>
+        <v>99794</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H22" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1587,10 +1574,10 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>725</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1599,10 +1586,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1613,10 +1600,10 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>809</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1625,10 +1612,10 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H24" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1639,22 +1626,22 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1665,10 +1652,10 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>253</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1677,10 +1664,10 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1691,10 +1678,10 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>55</v>
+        <v>178</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1703,10 +1690,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H27" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1717,22 +1704,22 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>157483</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H28" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1743,22 +1730,22 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>6473</v>
+        <v>1183</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H29" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1769,10 +1756,10 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1781,10 +1768,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H30" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1795,22 +1782,22 @@
         <v>36</v>
       </c>
       <c r="C31">
-        <v>111</v>
+        <v>486</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H31" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1821,10 +1808,10 @@
         <v>37</v>
       </c>
       <c r="C32">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1833,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H32" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1847,22 +1834,22 @@
         <v>38</v>
       </c>
       <c r="C33">
-        <v>2280</v>
+        <v>135</v>
       </c>
       <c r="D33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H33" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1873,10 +1860,10 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>501</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1885,10 +1872,10 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H34" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1899,10 +1886,10 @@
         <v>40</v>
       </c>
       <c r="C35">
-        <v>2099</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1911,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H35" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1925,22 +1912,22 @@
         <v>41</v>
       </c>
       <c r="C36">
-        <v>4245</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="H36" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1951,22 +1938,22 @@
         <v>42</v>
       </c>
       <c r="C37">
-        <v>4245</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="H37" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1977,22 +1964,22 @@
         <v>43</v>
       </c>
       <c r="C38">
-        <v>816</v>
+        <v>1050</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H38" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2003,10 +1990,10 @@
         <v>44</v>
       </c>
       <c r="C39">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2015,10 +2002,10 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H39" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2029,10 +2016,10 @@
         <v>45</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2041,10 +2028,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H40" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2055,10 +2042,10 @@
         <v>46</v>
       </c>
       <c r="C41">
-        <v>54</v>
+        <v>6469</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2067,10 +2054,10 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H41" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2081,10 +2068,10 @@
         <v>47</v>
       </c>
       <c r="C42">
-        <v>17</v>
+        <v>215</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2093,10 +2080,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H42" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2107,10 +2094,10 @@
         <v>48</v>
       </c>
       <c r="C43">
-        <v>2173</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2119,10 +2106,10 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H43" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2133,10 +2120,10 @@
         <v>49</v>
       </c>
       <c r="C44">
-        <v>83</v>
+        <v>423</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2145,10 +2132,10 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H44" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2159,13 +2146,13 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>17</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -2174,7 +2161,7 @@
         <v>134</v>
       </c>
       <c r="H45" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2185,10 +2172,10 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>3141</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2197,24 +2184,24 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="H46" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>52</v>
       </c>
       <c r="C47">
-        <v>346</v>
+        <v>4117</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2223,10 +2210,10 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H47" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2237,10 +2224,10 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>4725</v>
+        <v>999</v>
       </c>
       <c r="D48" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2249,10 +2236,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H48" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2263,10 +2250,10 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>3141</v>
+        <v>94</v>
       </c>
       <c r="D49" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2275,10 +2262,10 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H49" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2289,10 +2276,10 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2301,10 +2288,10 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H50" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2315,10 +2302,10 @@
         <v>56</v>
       </c>
       <c r="C51">
-        <v>798</v>
+        <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2327,16 +2314,15 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H51" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" location="Tesla%20#TSLA%20#TeslaStock%20#ElonMusk%20https://t.co/oAZUz2vQmM"/>
-    <hyperlink ref="B47" r:id="rId2" location="SPY%20#TSLA%20$MULN"/>
+    <hyperlink ref="B22" r:id="rId1" location="Tesla%20#TSLA%20#TeslaStock%20#ElonMusk%20#SenatorKaren%20https://t.co/2Ah7lBRlXl"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Twitter Streamer, Keywordsearch and ListToDF with CleanDates func
</commit_message>
<xml_diff>
--- a/docs/datasets/tweet_dataset.xlsx
+++ b/docs/datasets/tweet_dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="186">
   <si>
     <t>Tweet</t>
   </si>
@@ -35,6 +35,148 @@
   </si>
   <si>
     <t>Hashtags</t>
+  </si>
+  <si>
+    <t>#RIVN #TSLA #FSR #AAPL #MSFT #XPEV #NIO #AMZN #Bitcoin #EV #AMC #GME  #BTC #cryptocurrency #Ethereum #XRP  #doge #LCID $LCID 
+IMO. AMAZON is buying #MULN $MULN EV delivery vans this Q2 2022.
+Rivian $RIVN failed to deliver and has lower range compared to MULLEN EV vans.</t>
+  </si>
+  <si>
+    <t>The biggest bear trap in history I love it 
+#tsla #amzn #shop</t>
+  </si>
+  <si>
+    <t>Check out my #TSLA analysis on @TradingView: https://t.co/1YfuZDuIRd</t>
+  </si>
+  <si>
+    <t>The best live room community here at TradeEZ #DayTrading $TSLA #tsla https://t.co/QXizdY13hN</t>
+  </si>
+  <si>
+    <t>$TSLA #TSLA Potential 1D bull flag. 
+Bulls must keep the pullback healthy by holding 1053.60. Below is a gap fill to 1025ish and could see a bigger drop.
+Watching to see if 1h RSI touching 30 (~1060) results in a notable bounce.
+Key resist 1115 for a bull break #stockstowatch https://t.co/aZliQa2Yah</t>
+  </si>
+  <si>
+    <t>$RBLX TOP 10 STOCKS TO OWN APRIL 2022 - RICH TV LIVE https://t.co/qtpeThOIUW via  
+@YouTube 
+ #TOP10 #STOCKS #RICHTVLIVE #TRADING #BUSINESS #NEWS #FINANCE #EDUCATION #MONEY #WIN #AMZN #GOOG #TSLA #RBLX #richpicksdaily #richtv 
+https://t.co/iaQXxIYniS</t>
+  </si>
+  <si>
+    <t>@KrestTest @GerberKawasaki @TroyTeslike announcement will surprise #TSLA bounce back on April 4th for sure!!! https://t.co/s3qTpn3lbq</t>
+  </si>
+  <si>
+    <t>#tsla down 1% but let’s not forget them says it pushed over 50% ⛽️⛽️⛽️⛽️⛽️🚀🚀🚀🚀 just want to see this stock out smoke all the other cars 🚗 https://t.co/wXnB5p0ToN</t>
+  </si>
+  <si>
+    <t>Check out my new NFT on OpenSea! https://t.co/JXmI39USKZ via @opensea #NFT #NFTCommmunity #opensea #rich #richtv #richtvlive #richpicksdaily #richpicksdaily #amzn #rblx #goog #tsla #fedex</t>
+  </si>
+  <si>
+    <t>@jimcramer what’s your call on #tsla would like to know where you see it going today….  @elonmusk https://t.co/WwntWdGx93</t>
+  </si>
+  <si>
+    <t>#gme up 8% on the day #tsla. Looking like a fish out of water right now 
+With red  na s’more coming #puts like I been saying for 3days 🤑. It’s getting a lil weird now so I’m all out 🤦🏻‍♂️ take what I could make 🎯 #gme still in for bigger gains to come</t>
+  </si>
+  <si>
+    <t>“I don’t care that they stole my invention-I care that they don’t understand my invention” Nikola Tesla #cro #Croatia #Serbian #Elon #$TSLA #dogecoin #TSLA #dogearmy #Robinhood #doge #SHIB #DogecoinToTheMoon #$TSLA #SHIBARMY #cryptotax #Crypto now why is your sorry ass @elonmusk https://t.co/Rz2yJyJ29M</t>
+  </si>
+  <si>
+    <t>Who’s in on #tsla puts 🤑</t>
+  </si>
+  <si>
+    <t>TOP 10 STOCKS TO OWN APRIL 2022 - RICH TV LIVE https://t.co/qtpeTi6jMu via @YouTube #TOP10 #STOCKS #RICHTVLIVE #TRADING #BUSINESS #NEWS #FINANCE #EDUCATION #MONEY #WIN #AMZN #GOOG #TSLA #RBLX #richpicksdaily #richtv</t>
+  </si>
+  <si>
+    <t>#TSLA looks like it’s hanging on by a thread..</t>
+  </si>
+  <si>
+    <t>Hey @elonmusk , this is day 4 of asking how I should go about getting an engineering career in @Tesla 🤷🏻‍♂️ #Tesla #ElonMusk #SpaceX #TSLA #Starlink #FutureMillionare</t>
+  </si>
+  <si>
+    <t>Stock Market Timing 20220401 #SPY #DIA #QQQ #TSX #TSX_60 #VIX #WEED #CAT #TSLA #Trading https://t.co/kA1KDpjw7u</t>
+  </si>
+  <si>
+    <t>3/31 Daily Watchlist Recap #TSLA #AAPL #ABNB #FB #MSFT #TGT #OptionsTrading #DayTrading https://t.co/vxDgQipKim</t>
+  </si>
+  <si>
+    <t>Stocks Picks of the Day 
+#BIDU -long 
+#BABA -long 
+#PDD -long 
+ #TSLA -long #stockmarket #stocks #tranding #tiktok #fypシ #viral #fanpage https://t.co/6pLBKxMe2S</t>
+  </si>
+  <si>
+    <t>This is a fantastic video showing the #Gigafactory which is a system of systems producing a system (car) #TSLA https://t.co/nVqx4vQCw1</t>
+  </si>
+  <si>
+    <t>#RIVN #TSLA #FSR #AAPL #MSFT #XPEV #NIO #AMZN #Bitcoin #EV #AMC #GME  #BTC #cryptocurrency #Ethereum #XRP  #doge #LCID $LCID 
+#MULN $MULN is on 🔥
+https://t.co/ZUCutm4IIK</t>
+  </si>
+  <si>
+    <t>If #tsla moves up I sale my puts . If #tsla goes down I sale my call . Either way #tsla going print for me</t>
+  </si>
+  <si>
+    <t>@ShibaMyInu Yess Yesss !!! Perseverance my friend will guarantee a successful end ! #DogecoinToTheMoon #doge # $DOGE #TSLA # $TSLA  #shib #godisgood #FridayVibes #FridayThoughts #ETH #Ethereum #Bitcoin #Robinhood #HODL #SHIBARMY #Coinbase Have a nice day my friends 😘💯 https://t.co/YpuAO9EYQL</t>
+  </si>
+  <si>
+    <t>#RIVN #TSLA #FSR #AAPL #MSFT #XPEV #NIO #AMZN #Bitcoin #EV #AMC #GME  #BTC #cryptocurrency #Ethereum #XRP  #doge #LCID $LCID 
+A Fortune 500 company is buying #MULN $MULN EV delivery vans Q2 2022.
+Will MULN reclaim $15 or higher in a few weeks?
+https://t.co/ExSa80J13T</t>
+  </si>
+  <si>
+    <t>#TSLA  looks like it’s heading  back to a blood bath dump $1067/$1058 $1024/ $1017
+If it pass and holds $1096 /$1100/$1156/ $1208 /$1230 
+But the chart around ball park I’m just going sit in my hands till gaps get filled and better support come 🎯👀  @elonmusk  still a Genius https://t.co/fjMoFdRRdV</t>
+  </si>
+  <si>
+    <t>F! Looks like my Tesla ride is over RIP - 2019 P3D FSD plate STARSHP! 
+Going to sell the car for scrap and unload all my TSLA
+The growth story is busted!
+@WholeMarsBlog @DriveTeslaca #tsla #tesla #fwaud https://t.co/kgJFefDYsV</t>
+  </si>
+  <si>
+    <t>@elonmusk asked us to list #Tesla (#TSLA) on #KickEX. Should we list it?</t>
+  </si>
+  <si>
+    <t>📈Breaking @Tesla announces #FSD wide release to all US #Tesla owners with free one month trial for new users. 
+#tsla 
+#BREAKING</t>
+  </si>
+  <si>
+    <t>Want those rims for my Model X 😍⁦@Tesla⁩ ⁦@elonmusk⁩ #TSLA
+Star Trek: Picard
+S02E05 https://t.co/KXfutnXvcd</t>
+  </si>
+  <si>
+    <t>“A lot about having a car, it’s about freedom, it’s about going where you want to go” @elonmusk 
+#tsla #supercharging 
+https://t.co/vFLeUEIG5G</t>
+  </si>
+  <si>
+    <t>@elonmusk  #tsla not looking good for the day  but hold and long looks good after the blood bath https://t.co/815yrD6kZV</t>
+  </si>
+  <si>
+    <t>#TSLA holds the key technologies needed to mass produce a bot for the usages pursued because of their research &amp;amp; capabilities behind FSD. $TSLA will moon the day this occurs. Can’t afford not to be invested! Here’s a video I did taking a deeper dive.
+https://t.co/m5W87NFzcG</t>
+  </si>
+  <si>
+    <t>#tsla #gme #amc #amd let’s gooo locking in some buys to hold 🎯🤑🚀😍</t>
+  </si>
+  <si>
+    <t>#RIVN #TSLA #FSR #AAPL #MSFT #XPEV #NIO #AMZN #Bitcoin #EV #AMC #GME  #BTC #cryptocurrency #Ethereum #XRP  #doge #LCID $LCID 
+We are officially on Q2 2022.
+A big Fortune 500 company is buying #MULN $MULN EV delivery vans Q2 2022.
+Will MULN reclaim $15 in a few weeks?</t>
+  </si>
+  <si>
+    <t>#RIVN #TSLA #FSR #AAPL #MSFT #XPEV #NIO #AMZN #Bitcoin #EV #AMC #GME  #BTC #cryptocurrency #Ethereum #XRP  #doge #LCID $LCID 
+We are officially on Q2 2022.
+Which big Fortune 500 company buying #MULN $MULN EV delivery vans Q2 2022 as MULLEN CEO mentioned 2 days ago
+VOTE👇 https://t.co/V7Ekec4DES</t>
   </si>
   <si>
     <t>We wish you more Bitcoins and...healthy fruits in April 😄
@@ -94,143 +236,100 @@
     <t>@RedTeslaGirl @matthew35746729 @Jefferies @Yahoo @Tesla The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
   </si>
   <si>
-    <t>@financiahlth @YouTube The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@eltroglograd @Tesla The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@shanthirex The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@Moshkelgosha_M The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@EXOTICSPEED The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>https://t.co/WUHbGSrydG - Tesla “Defying Gravity” As Karen Attacks &amp;amp; TIME Snubs
-NEW
-$TSLA #Tesla #TSLA #TeslaStock #ElonMusk #SenatorKaren https://t.co/2Ah7lBRlXl</t>
-  </si>
-  <si>
-    <t>#TSLA My track record shows I know when to short Tesla ..! https://t.co/HaiXfMhyJp</t>
-  </si>
-  <si>
-    <t>$TSLA HP bounce zone at confluence of flag bottom and support around 1070 .
-Also can reject at 1090 .
-Calls above 1090 if it breaks with PT at 1100.
-#TSLA #Tesla #ElonMusk #ChartoftheDay #options #ElectricVehicles https://t.co/HUoyLIGU79</t>
-  </si>
-  <si>
-    <t>$TSLA 👀 Forming a bull flag after it rejected off 1115- 1120 zone. 
-If 1070 breaks, then PTs are 1055 and 1040 for sure.
-#Tesla #ElonMusk #TSLA #Tradeidea #optionstrade #ElectricVehicles #Bullish https://t.co/WXULCfUr2U</t>
-  </si>
-  <si>
-    <t>@teslaownersSV @elonmusk Me tomorrow morning after I tell work I’m sick…Sick of working there cause 🩳  ARE GONNA EAT CROW!! #MOASS #GME #AMC #TSLA #HYMC</t>
-  </si>
-  <si>
-    <t>@VoltBossBaby @ShibaArchives $Volt is going to be parabolic soon #VOLT #VOLTINU #VOLTARMY #ETH #BNB #TSLA @VoltInuOfficial @VoltArmy_ @cz_binance @ChinaPumpCN @elonmusk @VitalikButerin @pablo_cro @TheGen35 @icryptocare @LuckyTruong75 https://t.co/EEPqaR80NK</t>
-  </si>
-  <si>
-    <t>Domain Name For Sale
-https://t.co/efsHn3CsYl
-.
-#Domains #domainnameforsale #domainsforsale #cryptocurrency #Coinbase  #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3Coin #DAO https://t.co/9cfNugucOk</t>
-  </si>
-  <si>
-    <t>$TSLA $NIO $XPEV $LI.. all eyes on supply chain/production as EV makers prepare to release quarterly deliveries..
-https://t.co/4qz8rp7FzP
-#tsla #teslastock #tesla #nio #niostock #marchquarterdeliveries</t>
-  </si>
-  <si>
-    <t>@Tesla #TSLA short. This technology is insane and unsustainable. Besides what if you have a disagreement with the owner. He can shut your car down! https://t.co/nQR34bA1Jh</t>
-  </si>
-  <si>
-    <t>FREE WATCHLIST WIH ENTRY PRICE AND PRICE TARGETS 
-#tsla #twtr #snap #snow $snow $tsa $snap 
-$twtr #gme #amc $gme $amc https://t.co/YpJ1Zm45dq</t>
-  </si>
-  <si>
-    <t>#tesla #tsla Tesla $1150 Monday after q1 deliveries on the weekend, tesla $1250 all time high Friday with Texas party opening. Possible?</t>
-  </si>
-  <si>
-    <t>$TSLA gappy-gap-gap
-#optionflow #StockMarket #OptionsTrading #options #wallstreet #Daytrade #stocks #tsla https://t.co/DQ0Du3LQWX</t>
-  </si>
-  <si>
-    <t>#TSLA puts?? 🧐 https://t.co/VaEPrXiL8A</t>
-  </si>
-  <si>
-    <t>@srj5679 @jimcramer If Cramer says it gonna tank, better go all-in. That’s what Ive learned. #TSLA</t>
-  </si>
-  <si>
-    <t>Domain Name For Sale
-https://t.co/EOQhFILek7
-.
-#Domains #domainnameforsale #domainsforsale #cryptocurrency #cryptotrading #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3Coin https://t.co/ibXs7a4rcM</t>
-  </si>
-  <si>
-    <t>Domain Name For Sale
-https://t.co/gsVU2vOJcc
-.
-#Domains #domainnameforsale #domainsforsale #cryptocurrency #cryptotrading #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3 #Wallet https://t.co/URx52bOp2n</t>
-  </si>
-  <si>
-    <t>$tsla #TSLA | D | Hit 2nd ring #geocharting #marketgeometry #nextgentools #gocharting https://t.co/XvnHPlSAen</t>
-  </si>
-  <si>
-    <t>@cbcmarketplace Interesting… just wondering, can a #tesla be stolen in the same fashion, too? No key holes, no push start button. #ElectricVehicles #TSLA @tesla @elonmusk https://t.co/FM8vx6VYEp</t>
-  </si>
-  <si>
-    <t>@matthew35746729 @Jefferies @Yahoo Absolutely Matthew!  #Tesla #Brother!  
-#TSLA @Tesla</t>
-  </si>
-  <si>
-    <t>$TSLA #TSLA no change here as IMO retrace should continue lower.
-R1 pivot $1065.20 and pwHighs $1040.70 to be tested with a gap to fill much lower. 
-Call volume has been outflowing. Waiting to see Put volume increase. 
-#stocks https://t.co/zw6Td9e5CI https://t.co/jf2qln7QPT</t>
-  </si>
-  <si>
-    <t>Report: Tesla Giga Shanghai Will Extend Plant Suspension #TSLA #ElonMusk #Tesla #Sustainability #SDGs [Video]: The Tesla Giga Shanghai plant has suspended production of electric cars for several days, but it might not be the end of COVID-19-related… https://t.co/MHDoOaKq5H https://t.co/QQ2CL496IH</t>
-  </si>
-  <si>
-    <t>Report: Tesla Giga Shanghai Will Extend Plant Suspension #TSLA #ElonMusk #Tesla #Sustainability #SDGs [Video]: The Tesla Giga Shanghai plant has suspended production of electric cars for several days, but it might not be the end of COVID-19-related… https://t.co/ZOHltlE5QL https://t.co/ILc6mUVeE5</t>
-  </si>
-  <si>
-    <t>Why do people sell their stocks?
-Cause they need money to buy the stocks at a higher price lol 🤣🤣🤣
-#Truestory $TSLA #TSLA</t>
-  </si>
-  <si>
-    <t>TESLA-SELL strategy - #TSLA chart on @TradingView https://t.co/mkyoAoFqqY</t>
-  </si>
-  <si>
-    <t>#TSLA going to 1095 in 5 days? Hopefully. https://t.co/bLeA9kSpUt</t>
-  </si>
-  <si>
-    <t>We are hosting our daily market charting workshop on Discord.
-In these workshop:
-1. We do technical analysis 📈
-2. Plan our trades for coming days ✍️
-3. Q&amp;amp;A with our members 🗣️
-Try it for yourself with a 3-day Risk free trial:
-https://t.co/EpGQOYlg7k
-#WallStreet #tsla #SPX #SPY https://t.co/6mdof3FAJ3</t>
-  </si>
-  <si>
-    <t>The price of a commodity will never go to zero. When you invest in commodities futures, you are not buying a piece of paper that says you own an intangible of the company that can go bankrupt. #AMZN #tsla #TradingView https://t.co/xzxrra8FRp</t>
-  </si>
-  <si>
-    <t>@GrunzkeLukas @DoctorJack16 The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk  #Monkeys  #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@DoctorJack16 #NIO not because they will overtake #TSLA per se, but with a 30 billion dollar market cap with a good chance to be the market leader in China (soon to be largest economy in the world), the upside is far greater imo</t>
-  </si>
-  <si>
-    <t>Serviced my 22 Model 3 for a rattle/squeak. Service was great, fast, got it done. @Tesla #tsla</t>
+    <t>01-04-2022 14:14</t>
+  </si>
+  <si>
+    <t>01-04-2022 14:09</t>
+  </si>
+  <si>
+    <t>01-04-2022 14:05</t>
+  </si>
+  <si>
+    <t>01-04-2022 14:02</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:59</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:58</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:56</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:52</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:47</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:41</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:36</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:32</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:30</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:24</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:14</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:07</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:06</t>
+  </si>
+  <si>
+    <t>01-04-2022 13:00</t>
+  </si>
+  <si>
+    <t>01-04-2022 12:58</t>
+  </si>
+  <si>
+    <t>01-04-2022 12:55</t>
+  </si>
+  <si>
+    <t>01-04-2022 12:50</t>
+  </si>
+  <si>
+    <t>01-04-2022 12:48</t>
+  </si>
+  <si>
+    <t>01-04-2022 12:45</t>
+  </si>
+  <si>
+    <t>01-04-2022 12:37</t>
+  </si>
+  <si>
+    <t>01-04-2022 11:50</t>
+  </si>
+  <si>
+    <t>01-04-2022 11:38</t>
+  </si>
+  <si>
+    <t>01-04-2022 11:36</t>
+  </si>
+  <si>
+    <t>01-04-2022 11:29</t>
+  </si>
+  <si>
+    <t>01-04-2022 11:28</t>
+  </si>
+  <si>
+    <t>01-04-2022 11:08</t>
+  </si>
+  <si>
+    <t>01-04-2022 10:50</t>
+  </si>
+  <si>
+    <t>01-04-2022 10:36</t>
   </si>
   <si>
     <t>01-04-2022 09:23</t>
@@ -278,91 +377,70 @@
     <t>01-04-2022 05:52</t>
   </si>
   <si>
-    <t>01-04-2022 05:51</t>
-  </si>
-  <si>
-    <t>01-04-2022 05:50</t>
-  </si>
-  <si>
-    <t>01-04-2022 05:30</t>
-  </si>
-  <si>
-    <t>01-04-2022 05:28</t>
-  </si>
-  <si>
-    <t>01-04-2022 04:52</t>
-  </si>
-  <si>
-    <t>01-04-2022 04:47</t>
-  </si>
-  <si>
-    <t>01-04-2022 04:46</t>
-  </si>
-  <si>
-    <t>01-04-2022 04:28</t>
-  </si>
-  <si>
-    <t>01-04-2022 04:00</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:59</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:37</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:29</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:25</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:24</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:19</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:18</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:15</t>
-  </si>
-  <si>
-    <t>01-04-2022 03:00</t>
-  </si>
-  <si>
-    <t>01-04-2022 02:33</t>
-  </si>
-  <si>
-    <t>01-04-2022 02:22</t>
-  </si>
-  <si>
-    <t>01-04-2022 02:17</t>
-  </si>
-  <si>
-    <t>01-04-2022 02:09</t>
-  </si>
-  <si>
-    <t>01-04-2022 01:18</t>
-  </si>
-  <si>
-    <t>01-04-2022 01:01</t>
-  </si>
-  <si>
-    <t>01-04-2022 00:42</t>
-  </si>
-  <si>
-    <t>01-04-2022 00:38</t>
-  </si>
-  <si>
-    <t>01-04-2022 00:24</t>
-  </si>
-  <si>
-    <t>01-04-2022 00:19</t>
-  </si>
-  <si>
-    <t>01-04-2022 00:00</t>
+    <t>16-09-2021 13:23</t>
+  </si>
+  <si>
+    <t>02-09-2020 15:23</t>
+  </si>
+  <si>
+    <t>04-06-2013 09:19</t>
+  </si>
+  <si>
+    <t>06-12-2017 18:09</t>
+  </si>
+  <si>
+    <t>20-02-2021 21:45</t>
+  </si>
+  <si>
+    <t>08-02-2013 15:56</t>
+  </si>
+  <si>
+    <t>25-03-2021 17:07</t>
+  </si>
+  <si>
+    <t>30-08-2011 12:26</t>
+  </si>
+  <si>
+    <t>19-10-2008 18:56</t>
+  </si>
+  <si>
+    <t>09-07-2021 21:38</t>
+  </si>
+  <si>
+    <t>12-05-2020 12:19</t>
+  </si>
+  <si>
+    <t>04-03-2009 21:58</t>
+  </si>
+  <si>
+    <t>12-08-2021 00:00</t>
+  </si>
+  <si>
+    <t>15-04-2016 14:42</t>
+  </si>
+  <si>
+    <t>14-04-2010 13:43</t>
+  </si>
+  <si>
+    <t>14-12-2017 14:31</t>
+  </si>
+  <si>
+    <t>10-08-2019 13:57</t>
+  </si>
+  <si>
+    <t>19-02-2012 10:25</t>
+  </si>
+  <si>
+    <t>30-08-2011 23:10</t>
+  </si>
+  <si>
+    <t>14-04-2009 04:06</t>
+  </si>
+  <si>
+    <t>01-03-2020 01:37</t>
+  </si>
+  <si>
+    <t>16-02-2021 15:51</t>
   </si>
   <si>
     <t>20-05-2018 10:40</t>
@@ -392,9 +470,6 @@
     <t>27-01-2019 23:03</t>
   </si>
   <si>
-    <t>30-08-2011 12:26</t>
-  </si>
-  <si>
     <t>20-07-2020 10:59</t>
   </si>
   <si>
@@ -404,82 +479,103 @@
     <t>06-12-2010 23:58</t>
   </si>
   <si>
-    <t>14-04-2009 23:28</t>
-  </si>
-  <si>
-    <t>21-10-2020 22:09</t>
-  </si>
-  <si>
-    <t>31-03-2022 02:51</t>
-  </si>
-  <si>
-    <t>02-03-2011 00:30</t>
-  </si>
-  <si>
-    <t>28-01-2022 23:19</t>
-  </si>
-  <si>
-    <t>08-02-2022 20:08</t>
-  </si>
-  <si>
-    <t>26-09-2016 18:29</t>
-  </si>
-  <si>
-    <t>01-03-2022 04:23</t>
-  </si>
-  <si>
-    <t>25-06-2010 17:56</t>
-  </si>
-  <si>
-    <t>03-11-2009 16:30</t>
-  </si>
-  <si>
-    <t>05-03-2017 02:14</t>
-  </si>
-  <si>
-    <t>09-01-2018 05:26</t>
-  </si>
-  <si>
-    <t>30-09-2014 21:51</t>
-  </si>
-  <si>
-    <t>08-07-2019 00:06</t>
-  </si>
-  <si>
-    <t>15-08-2021 22:14</t>
-  </si>
-  <si>
-    <t>21-11-2020 19:42</t>
-  </si>
-  <si>
-    <t>10-12-2016 04:42</t>
-  </si>
-  <si>
-    <t>08-09-2008 22:56</t>
-  </si>
-  <si>
-    <t>07-05-2020 18:13</t>
-  </si>
-  <si>
-    <t>08-04-2018 16:19</t>
-  </si>
-  <si>
-    <t>18-09-2010 07:23</t>
-  </si>
-  <si>
-    <t>18-03-2022 00:09</t>
-  </si>
-  <si>
-    <t>09-12-2013 22:25</t>
-  </si>
-  <si>
-    <t>04-11-2020 09:43</t>
-  </si>
-  <si>
-    <t>07-10-2016 06:39</t>
-  </si>
-  <si>
-    <t>09-08-2016 20:38</t>
+    <t>[{'text': 'RIVN', 'indices': [0, 5]}, {'text': 'TSLA', 'indices': [6, 11]}, {'text': 'FSR', 'indices': [12, 16]}, {'text': 'AAPL', 'indices': [17, 22]}, {'text': 'MSFT', 'indices': [23, 28]}, {'text': 'XPEV', 'indices': [29, 34]}, {'text': 'NIO', 'indices': [35, 39]}, {'text': 'AMZN', 'indices': [40, 45]}, {'text': 'Bitcoin', 'indices': [46, 54]}, {'text': 'EV', 'indices': [55, 58]}, {'text': 'AMC', 'indices': [59, 63]}, {'text': 'GME', 'indices': [64, 68]}, {'text': 'BTC', 'indices': [70, 74]}, {'text': 'cryptocurrency', 'indices': [75, 90]}, {'text': 'Ethereum', 'indices': [91, 100]}, {'text': 'XRP', 'indices': [101, 105]}, {'text': 'doge', 'indices': [107, 112]}, {'text': 'LCID', 'indices': [113, 118]}, {'text': 'MULN', 'indices': [149, 154]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [45, 50]}, {'text': 'amzn', 'indices': [51, 56]}, {'text': 'shop', 'indices': [57, 62]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [13, 18]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'DayTrading', 'indices': [45, 56]}, {'text': 'tsla', 'indices': [63, 68]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'stockstowatch', 'indices': [265, 279]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TOP10', 'indices': [94, 100]}, {'text': 'STOCKS', 'indices': [101, 108]}, {'text': 'RICHTVLIVE', 'indices': [109, 120]}, {'text': 'TRADING', 'indices': [121, 129]}, {'text': 'BUSINESS', 'indices': [130, 139]}, {'text': 'NEWS', 'indices': [140, 145]}, {'text': 'FINANCE', 'indices': [146, 154]}, {'text': 'EDUCATION', 'indices': [155, 165]}, {'text': 'MONEY', 'indices': [166, 172]}, {'text': 'WIN', 'indices': [173, 177]}, {'text': 'AMZN', 'indices': [178, 183]}, {'text': 'GOOG', 'indices': [184, 189]}, {'text': 'TSLA', 'indices': [190, 195]}, {'text': 'RBLX', 'indices': [196, 201]}, {'text': 'richpicksdaily', 'indices': [202, 217]}, {'text': 'richtv', 'indices': [218, 225]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [67, 72]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [0, 5]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'NFT', 'indices': [70, 74]}, {'text': 'NFTCommmunity', 'indices': [75, 89]}, {'text': 'opensea', 'indices': [90, 98]}, {'text': 'rich', 'indices': [99, 104]}, {'text': 'richtv', 'indices': [105, 112]}, {'text': 'richtvlive', 'indices': [113, 124]}, {'text': 'richpicksdaily', 'indices': [125, 140]}, {'text': 'richpicksdaily', 'indices': [141, 156]}, {'text': 'amzn', 'indices': [157, 162]}, {'text': 'rblx', 'indices': [163, 168]}, {'text': 'goog', 'indices': [169, 174]}, {'text': 'tsla', 'indices': [175, 180]}, {'text': 'fedex', 'indices': [181, 187]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [31, 36]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'gme', 'indices': [0, 4]}, {'text': 'tsla', 'indices': [22, 27]}, {'text': 'puts', 'indices': [100, 105]}, {'text': 'gme', 'indices': [213, 217]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'cro', 'indices': [104, 108]}, {'text': 'Croatia', 'indices': [109, 117]}, {'text': 'Serbian', 'indices': [118, 126]}, {'text': 'Elon', 'indices': [127, 132]}, {'text': 'dogecoin', 'indices': [140, 149]}, {'text': 'TSLA', 'indices': [150, 155]}, {'text': 'dogearmy', 'indices': [156, 165]}, {'text': 'Robinhood', 'indices': [166, 176]}, {'text': 'doge', 'indices': [177, 182]}, {'text': 'SHIB', 'indices': [183, 188]}, {'text': 'DogecoinToTheMoon', 'indices': [189, 207]}, {'text': 'SHIBARMY', 'indices': [215, 224]}, {'text': 'cryptotax', 'indices': [225, 235]}, {'text': 'Crypto', 'indices': [236, 243]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [12, 17]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TOP10', 'indices': [84, 90]}, {'text': 'STOCKS', 'indices': [91, 98]}, {'text': 'RICHTVLIVE', 'indices': [99, 110]}, {'text': 'TRADING', 'indices': [111, 119]}, {'text': 'BUSINESS', 'indices': [120, 129]}, {'text': 'NEWS', 'indices': [130, 135]}, {'text': 'FINANCE', 'indices': [136, 144]}, {'text': 'EDUCATION', 'indices': [145, 155]}, {'text': 'MONEY', 'indices': [156, 162]}, {'text': 'WIN', 'indices': [163, 167]}, {'text': 'AMZN', 'indices': [168, 173]}, {'text': 'GOOG', 'indices': [174, 179]}, {'text': 'TSLA', 'indices': [180, 185]}, {'text': 'RBLX', 'indices': [186, 191]}, {'text': 'richpicksdaily', 'indices': [192, 207]}, {'text': 'richtv', 'indices': [208, 215]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [0, 5]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [108, 114]}, {'text': 'ElonMusk', 'indices': [115, 124]}, {'text': 'SpaceX', 'indices': [125, 132]}, {'text': 'TSLA', 'indices': [133, 138]}, {'text': 'Starlink', 'indices': [139, 148]}, {'text': 'FutureMillionare', 'indices': [149, 166]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'SPY', 'indices': [29, 33]}, {'text': 'DIA', 'indices': [34, 38]}, {'text': 'QQQ', 'indices': [39, 43]}, {'text': 'TSX', 'indices': [44, 48]}, {'text': 'TSX_60', 'indices': [49, 56]}, {'text': 'VIX', 'indices': [57, 61]}, {'text': 'WEED', 'indices': [62, 67]}, {'text': 'CAT', 'indices': [68, 72]}, {'text': 'TSLA', 'indices': [73, 78]}, {'text': 'Trading', 'indices': [79, 87]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [27, 32]}, {'text': 'AAPL', 'indices': [33, 38]}, {'text': 'ABNB', 'indices': [39, 44]}, {'text': 'FB', 'indices': [45, 48]}, {'text': 'MSFT', 'indices': [49, 54]}, {'text': 'TGT', 'indices': [55, 59]}, {'text': 'OptionsTrading', 'indices': [60, 75]}, {'text': 'DayTrading', 'indices': [76, 87]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'BIDU', 'indices': [25, 30]}, {'text': 'BABA', 'indices': [38, 43]}, {'text': 'PDD', 'indices': [51, 55]}, {'text': 'TSLA', 'indices': [64, 69]}, {'text': 'stockmarket', 'indices': [76, 88]}, {'text': 'stocks', 'indices': [89, 96]}, {'text': 'tranding', 'indices': [97, 106]}, {'text': 'tiktok', 'indices': [107, 114]}, {'text': 'fypシ', 'indices': [115, 120]}, {'text': 'viral', 'indices': [121, 127]}, {'text': 'fanpage', 'indices': [128, 136]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Gigafactory', 'indices': [38, 50]}, {'text': 'TSLA', 'indices': [105, 110]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'RIVN', 'indices': [0, 5]}, {'text': 'TSLA', 'indices': [6, 11]}, {'text': 'FSR', 'indices': [12, 16]}, {'text': 'AAPL', 'indices': [17, 22]}, {'text': 'MSFT', 'indices': [23, 28]}, {'text': 'XPEV', 'indices': [29, 34]}, {'text': 'NIO', 'indices': [35, 39]}, {'text': 'AMZN', 'indices': [40, 45]}, {'text': 'Bitcoin', 'indices': [46, 54]}, {'text': 'EV', 'indices': [55, 58]}, {'text': 'AMC', 'indices': [59, 63]}, {'text': 'GME', 'indices': [64, 68]}, {'text': 'BTC', 'indices': [70, 74]}, {'text': 'cryptocurrency', 'indices': [75, 90]}, {'text': 'Ethereum', 'indices': [91, 100]}, {'text': 'XRP', 'indices': [101, 105]}, {'text': 'doge', 'indices': [107, 112]}, {'text': 'LCID', 'indices': [113, 118]}, {'text': 'MULN', 'indices': [127, 132]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [3, 8]}, {'text': 'tsla', 'indices': [38, 43]}, {'text': 'tsla', 'indices': [82, 87]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'DogecoinToTheMoon', 'indices': [84, 102]}, {'text': 'doge', 'indices': [103, 108]}, {'text': 'TSLA', 'indices': [117, 122]}, {'text': 'shib', 'indices': [132, 137]}, {'text': 'godisgood', 'indices': [138, 148]}, {'text': 'FridayVibes', 'indices': [149, 161]}, {'text': 'FridayThoughts', 'indices': [162, 177]}, {'text': 'ETH', 'indices': [178, 182]}, {'text': 'Ethereum', 'indices': [183, 192]}, {'text': 'Bitcoin', 'indices': [193, 201]}, {'text': 'Robinhood', 'indices': [202, 212]}, {'text': 'HODL', 'indices': [213, 218]}, {'text': 'SHIBARMY', 'indices': [219, 228]}, {'text': 'Coinbase', 'indices': [229, 238]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'RIVN', 'indices': [0, 5]}, {'text': 'TSLA', 'indices': [6, 11]}, {'text': 'FSR', 'indices': [12, 16]}, {'text': 'AAPL', 'indices': [17, 22]}, {'text': 'MSFT', 'indices': [23, 28]}, {'text': 'XPEV', 'indices': [29, 34]}, {'text': 'NIO', 'indices': [35, 39]}, {'text': 'AMZN', 'indices': [40, 45]}, {'text': 'Bitcoin', 'indices': [46, 54]}, {'text': 'EV', 'indices': [55, 58]}, {'text': 'AMC', 'indices': [59, 63]}, {'text': 'GME', 'indices': [64, 68]}, {'text': 'BTC', 'indices': [70, 74]}, {'text': 'cryptocurrency', 'indices': [75, 90]}, {'text': 'Ethereum', 'indices': [91, 100]}, {'text': 'XRP', 'indices': [101, 105]}, {'text': 'doge', 'indices': [107, 112]}, {'text': 'LCID', 'indices': [113, 118]}, {'text': 'MULN', 'indices': [159, 164]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [186, 191]}, {'text': 'tesla', 'indices': [192, 198]}, {'text': 'fwaud', 'indices': [199, 205]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [27, 33]}, {'text': 'TSLA', 'indices': [35, 40]}, {'text': 'KickEX', 'indices': [45, 52]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'FSD', 'indices': [27, 31]}, {'text': 'Tesla', 'indices': [55, 61]}, {'text': 'tsla', 'indices': [111, 116]}, {'text': 'BREAKING', 'indices': [118, 127]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [53, 58]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [97, 102]}, {'text': 'supercharging', 'indices': [103, 117]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [11, 16]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [0, 5]}, {'text': 'gme', 'indices': [6, 10]}, {'text': 'amc', 'indices': [11, 15]}, {'text': 'amd', 'indices': [16, 20]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'RIVN', 'indices': [0, 5]}, {'text': 'TSLA', 'indices': [6, 11]}, {'text': 'FSR', 'indices': [12, 16]}, {'text': 'AAPL', 'indices': [17, 22]}, {'text': 'MSFT', 'indices': [23, 28]}, {'text': 'XPEV', 'indices': [29, 34]}, {'text': 'NIO', 'indices': [35, 39]}, {'text': 'AMZN', 'indices': [40, 45]}, {'text': 'Bitcoin', 'indices': [46, 54]}, {'text': 'EV', 'indices': [55, 58]}, {'text': 'AMC', 'indices': [59, 63]}, {'text': 'GME', 'indices': [64, 68]}, {'text': 'BTC', 'indices': [70, 74]}, {'text': 'cryptocurrency', 'indices': [75, 90]}, {'text': 'Ethereum', 'indices': [91, 100]}, {'text': 'XRP', 'indices': [101, 105]}, {'text': 'doge', 'indices': [107, 112]}, {'text': 'LCID', 'indices': [113, 118]}, {'text': 'MULN', 'indices': [193, 198]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'RIVN', 'indices': [0, 5]}, {'text': 'TSLA', 'indices': [6, 11]}, {'text': 'FSR', 'indices': [12, 16]}, {'text': 'AAPL', 'indices': [17, 22]}, {'text': 'MSFT', 'indices': [23, 28]}, {'text': 'XPEV', 'indices': [29, 34]}, {'text': 'NIO', 'indices': [35, 39]}, {'text': 'AMZN', 'indices': [40, 45]}, {'text': 'Bitcoin', 'indices': [46, 54]}, {'text': 'EV', 'indices': [55, 58]}, {'text': 'AMC', 'indices': [59, 63]}, {'text': 'GME', 'indices': [64, 68]}, {'text': 'BTC', 'indices': [70, 74]}, {'text': 'cryptocurrency', 'indices': [75, 90]}, {'text': 'Ethereum', 'indices': [91, 100]}, {'text': 'XRP', 'indices': [101, 105]}, {'text': 'doge', 'indices': [107, 112]}, {'text': 'LCID', 'indices': [113, 118]}, {'text': 'MULN', 'indices': [194, 199]}]</t>
   </si>
   <si>
     <t>[{'text': 'newmonth', 'indices': [59, 68]}, {'text': 'bitcoin', 'indices': [69, 77]}, {'text': 'ethereum', 'indices': [78, 87]}, {'text': 'btc', 'indices': [88, 92]}, {'text': 'satoshi', 'indices': [93, 101]}, {'text': 'cryptonews', 'indices': [102, 113]}, {'text': 'binance', 'indices': [114, 122]}, {'text': 'satoshinakamoto', 'indices': [123, 139]}, {'text': 'btcmemes', 'indices': [140, 149]}, {'text': 'tsla', 'indices': [150, 155]}, {'text': 'wallstreetbets', 'indices': [156, 171]}, {'text': 'metaverse', 'indices': [172, 182]}, {'text': 'defi', 'indices': [183, 188]}, {'text': 'nft', 'indices': [189, 193]}, {'text': 'dogecoin', 'indices': [194, 203]}]</t>
@@ -525,109 +621,13 @@
   </si>
   <si>
     <t>[{'text': 'Musk', 'indices': [123, 128]}, {'text': 'ElonMusk', 'indices': [129, 138]}, {'text': 'Monkeys', 'indices': [140, 148]}, {'text': 'TSLA', 'indices': [150, 155]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [90, 95]}, {'text': 'ElonMusk', 'indices': [96, 105]}, {'text': 'Monkeys', 'indices': [107, 115]}, {'text': 'TSLA', 'indices': [117, 122]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [88, 93]}, {'text': 'ElonMusk', 'indices': [94, 103]}, {'text': 'Monkeys', 'indices': [105, 113]}, {'text': 'TSLA', 'indices': [115, 120]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [79, 84]}, {'text': 'ElonMusk', 'indices': [85, 94]}, {'text': 'Monkeys', 'indices': [96, 104]}, {'text': 'TSLA', 'indices': [106, 111]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [83, 88]}, {'text': 'ElonMusk', 'indices': [89, 98]}, {'text': 'Monkeys', 'indices': [100, 108]}, {'text': 'TSLA', 'indices': [110, 115]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [80, 85]}, {'text': 'ElonMusk', 'indices': [86, 95]}, {'text': 'Monkeys', 'indices': [97, 105]}, {'text': 'TSLA', 'indices': [107, 112]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [96, 102]}, {'text': 'TSLA', 'indices': [103, 108]}, {'text': 'TeslaStock', 'indices': [109, 120]}, {'text': 'ElonMusk', 'indices': [121, 130]}, {'text': 'SenatorKaren', 'indices': [131, 144]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [0, 5]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [149, 154]}, {'text': 'Tesla', 'indices': [155, 161]}, {'text': 'ElonMusk', 'indices': [162, 171]}, {'text': 'ChartoftheDay', 'indices': [172, 186]}, {'text': 'options', 'indices': [187, 195]}, {'text': 'ElectricVehicles', 'indices': [196, 213]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [121, 127]}, {'text': 'ElonMusk', 'indices': [128, 137]}, {'text': 'TSLA', 'indices': [138, 143]}, {'text': 'Tradeidea', 'indices': [144, 154]}, {'text': 'optionstrade', 'indices': [155, 168]}, {'text': 'ElectricVehicles', 'indices': [169, 186]}, {'text': 'Bullish', 'indices': [187, 195]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'MOASS', 'indices': [124, 130]}, {'text': 'GME', 'indices': [131, 135]}, {'text': 'AMC', 'indices': [136, 140]}, {'text': 'TSLA', 'indices': [141, 146]}, {'text': 'HYMC', 'indices': [147, 152]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'VOLT', 'indices': [65, 70]}, {'text': 'VOLTINU', 'indices': [71, 79]}, {'text': 'VOLTARMY', 'indices': [80, 89]}, {'text': 'ETH', 'indices': [90, 94]}, {'text': 'BNB', 'indices': [95, 99]}, {'text': 'TSLA', 'indices': [100, 105]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'Coinbase', 'indices': [107, 116]}, {'text': 'Crypto', 'indices': [118, 125]}, {'text': 'Cryptos', 'indices': [126, 134]}, {'text': 'cryptogiveaway', 'indices': [135, 150]}, {'text': 'CryptocurrencyNews', 'indices': [151, 170]}, {'text': 'Bitcoin', 'indices': [171, 179]}, {'text': 'cryptobank', 'indices': [180, 191]}, {'text': 'cryptowallet', 'indices': [192, 205]}, {'text': 'BTC', 'indices': [206, 210]}, {'text': 'Ethereum', 'indices': [211, 220]}, {'text': 'ETH', 'indices': [221, 225]}, {'text': 'tezos', 'indices': [226, 232]}, {'text': 'doge', 'indices': [233, 238]}, {'text': 'TSLA', 'indices': [239, 244]}, {'text': 'NFT', 'indices': [245, 249]}, {'text': 'blockchain', 'indices': [250, 261]}, {'text': 'Web3Coin', 'indices': [262, 271]}, {'text': 'DAO', 'indices': [272, 276]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [140, 145]}, {'text': 'teslastock', 'indices': [146, 157]}, {'text': 'tesla', 'indices': [158, 164]}, {'text': 'nio', 'indices': [165, 169]}, {'text': 'niostock', 'indices': [170, 179]}, {'text': 'marchquarterdeliveries', 'indices': [180, 203]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [7, 12]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [50, 55]}, {'text': 'twtr', 'indices': [56, 61]}, {'text': 'snap', 'indices': [62, 67]}, {'text': 'snow', 'indices': [68, 73]}, {'text': 'gme', 'indices': [98, 102]}, {'text': 'amc', 'indices': [103, 107]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tesla', 'indices': [0, 6]}, {'text': 'tsla', 'indices': [7, 12]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'optionflow', 'indices': [21, 32]}, {'text': 'StockMarket', 'indices': [33, 45]}, {'text': 'OptionsTrading', 'indices': [46, 61]}, {'text': 'options', 'indices': [62, 70]}, {'text': 'wallstreet', 'indices': [71, 82]}, {'text': 'Daytrade', 'indices': [83, 92]}, {'text': 'stocks', 'indices': [93, 100]}, {'text': 'tsla', 'indices': [101, 106]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [93, 98]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'cryptotrading', 'indices': [107, 121]}, {'text': 'Crypto', 'indices': [122, 129]}, {'text': 'Cryptos', 'indices': [130, 138]}, {'text': 'cryptogiveaway', 'indices': [139, 154]}, {'text': 'CryptocurrencyNews', 'indices': [155, 174]}, {'text': 'Bitcoin', 'indices': [175, 183]}, {'text': 'cryptobank', 'indices': [184, 195]}, {'text': 'cryptowallet', 'indices': [196, 209]}, {'text': 'BTC', 'indices': [210, 214]}, {'text': 'Ethereum', 'indices': [215, 224]}, {'text': 'ETH', 'indices': [225, 229]}, {'text': 'tezos', 'indices': [230, 236]}, {'text': 'doge', 'indices': [237, 242]}, {'text': 'TSLA', 'indices': [243, 248]}, {'text': 'NFT', 'indices': [249, 253]}, {'text': 'blockchain', 'indices': [254, 265]}, {'text': 'Web3Coin', 'indices': [266, 275]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'cryptotrading', 'indices': [107, 121]}, {'text': 'Crypto', 'indices': [122, 129]}, {'text': 'Cryptos', 'indices': [130, 138]}, {'text': 'cryptogiveaway', 'indices': [139, 154]}, {'text': 'CryptocurrencyNews', 'indices': [155, 174]}, {'text': 'Bitcoin', 'indices': [175, 183]}, {'text': 'cryptobank', 'indices': [184, 195]}, {'text': 'cryptowallet', 'indices': [196, 209]}, {'text': 'BTC', 'indices': [210, 214]}, {'text': 'Ethereum', 'indices': [215, 224]}, {'text': 'ETH', 'indices': [225, 229]}, {'text': 'tezos', 'indices': [230, 236]}, {'text': 'doge', 'indices': [237, 242]}, {'text': 'TSLA', 'indices': [243, 248]}, {'text': 'NFT', 'indices': [249, 253]}, {'text': 'blockchain', 'indices': [254, 265]}, {'text': 'Web3', 'indices': [266, 271]}, {'text': 'Wallet', 'indices': [272, 279]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'geocharting', 'indices': [31, 43]}, {'text': 'marketgeometry', 'indices': [44, 59]}, {'text': 'nextgentools', 'indices': [60, 73]}, {'text': 'gocharting', 'indices': [74, 85]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tesla', 'indices': [51, 57]}, {'text': 'ElectricVehicles', 'indices': [130, 147]}, {'text': 'TSLA', 'indices': [148, 153]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [56, 62]}, {'text': 'Brother', 'indices': [63, 71]}, {'text': 'TSLA', 'indices': [76, 81]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [6, 11]}, {'text': 'stocks', 'indices': [222, 229]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [57, 62]}, {'text': 'ElonMusk', 'indices': [63, 72]}, {'text': 'Tesla', 'indices': [73, 79]}, {'text': 'Sustainability', 'indices': [80, 95]}, {'text': 'SDGs', 'indices': [96, 101]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Truestory', 'indices': [101, 111]}, {'text': 'TSLA', 'indices': [118, 123]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [22, 27]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'WallStreet', 'indices': [255, 266]}, {'text': 'tsla', 'indices': [267, 272]}, {'text': 'SPX', 'indices': [273, 277]}, {'text': 'SPY', 'indices': [278, 282]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'AMZN', 'indices': [193, 198]}, {'text': 'tsla', 'indices': [199, 204]}, {'text': 'TradingView', 'indices': [205, 217]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [95, 100]}, {'text': 'ElonMusk', 'indices': [101, 110]}, {'text': 'Monkeys', 'indices': [112, 120]}, {'text': 'TSLA', 'indices': [122, 127]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'NIO', 'indices': [14, 18]}, {'text': 'TSLA', 'indices': [50, 55]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [89, 94]}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,13 +642,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -683,22 +676,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1028,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>8514</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1040,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1054,11 +1041,11 @@
         <v>8</v>
       </c>
       <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
       <c r="E3">
         <v>0</v>
       </c>
@@ -1066,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1080,22 +1067,22 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>460</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1106,10 +1093,10 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>5608</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1118,10 +1105,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1132,22 +1119,22 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>224</v>
+        <v>2906</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1158,22 +1145,22 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>38</v>
+        <v>1990</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1184,22 +1171,22 @@
         <v>13</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" t="s">
         <v>144</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1210,10 +1197,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>329</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1222,10 +1209,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1236,13 +1223,13 @@
         <v>15</v>
       </c>
       <c r="C10">
+        <v>1990</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10">
         <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1251,7 +1238,7 @@
         <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1265,7 +1252,7 @@
         <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1274,10 +1261,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1288,10 +1275,10 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1303,7 +1290,7 @@
         <v>111</v>
       </c>
       <c r="H12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1314,10 +1301,10 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>3140</v>
+        <v>1957</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1329,7 +1316,7 @@
         <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1343,7 +1330,7 @@
         <v>149</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1352,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1366,22 +1353,22 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>149</v>
+        <v>1990</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1392,10 +1379,10 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1407,7 +1394,7 @@
         <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1418,10 +1405,10 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1430,10 +1417,10 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1444,22 +1431,22 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>94</v>
+        <v>866</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1470,10 +1457,10 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1482,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1496,10 +1483,10 @@
         <v>25</v>
       </c>
       <c r="C20">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1508,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1522,7 +1509,7 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <v>94</v>
+        <v>485</v>
       </c>
       <c r="D21" t="s">
         <v>73</v>
@@ -1534,36 +1521,36 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>27</v>
       </c>
       <c r="C22">
-        <v>99794</v>
+        <v>195</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
       </c>
       <c r="E22">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1574,7 +1561,7 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>725</v>
+        <v>149</v>
       </c>
       <c r="D23" t="s">
         <v>75</v>
@@ -1586,10 +1573,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1600,22 +1587,22 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>1266</v>
       </c>
       <c r="D24" t="s">
         <v>76</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1626,7 +1613,7 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>195</v>
       </c>
       <c r="D25" t="s">
         <v>77</v>
@@ -1638,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1652,7 +1639,7 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>253</v>
+        <v>149</v>
       </c>
       <c r="D26" t="s">
         <v>78</v>
@@ -1664,10 +1651,10 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H26" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1678,7 +1665,7 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>178</v>
+        <v>231</v>
       </c>
       <c r="D27" t="s">
         <v>79</v>
@@ -1690,10 +1677,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1704,22 +1691,22 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>36</v>
+        <v>15230</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1730,22 +1717,22 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>1183</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>81</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H29" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1756,7 +1743,7 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
         <v>82</v>
@@ -1768,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1782,22 +1769,22 @@
         <v>36</v>
       </c>
       <c r="C31">
-        <v>486</v>
+        <v>43446</v>
       </c>
       <c r="D31" t="s">
         <v>83</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1808,7 +1795,7 @@
         <v>37</v>
       </c>
       <c r="C32">
-        <v>219</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
         <v>84</v>
@@ -1820,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="H32" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1834,7 +1821,7 @@
         <v>38</v>
       </c>
       <c r="C33">
-        <v>135</v>
+        <v>2044</v>
       </c>
       <c r="D33" t="s">
         <v>85</v>
@@ -1846,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H33" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1860,7 +1847,7 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>501</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
         <v>86</v>
@@ -1872,10 +1859,10 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="H34" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1886,7 +1873,7 @@
         <v>40</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>195</v>
       </c>
       <c r="D35" t="s">
         <v>87</v>
@@ -1898,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="H35" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1912,22 +1899,22 @@
         <v>41</v>
       </c>
       <c r="C36">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="D36" t="s">
         <v>88</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="H36" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1938,22 +1925,22 @@
         <v>42</v>
       </c>
       <c r="C37">
-        <v>36</v>
+        <v>8512</v>
       </c>
       <c r="D37" t="s">
         <v>89</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="H37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1964,13 +1951,13 @@
         <v>43</v>
       </c>
       <c r="C38">
-        <v>1050</v>
+        <v>57</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -1979,7 +1966,7 @@
         <v>127</v>
       </c>
       <c r="H38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1990,13 +1977,13 @@
         <v>44</v>
       </c>
       <c r="C39">
-        <v>27</v>
+        <v>460</v>
       </c>
       <c r="D39" t="s">
         <v>91</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -2005,7 +1992,7 @@
         <v>128</v>
       </c>
       <c r="H39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2016,7 +2003,7 @@
         <v>45</v>
       </c>
       <c r="C40">
-        <v>151</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
         <v>92</v>
@@ -2031,7 +2018,7 @@
         <v>129</v>
       </c>
       <c r="H40" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2042,10 +2029,10 @@
         <v>46</v>
       </c>
       <c r="C41">
-        <v>6469</v>
+        <v>224</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2057,7 +2044,7 @@
         <v>130</v>
       </c>
       <c r="H41" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2068,10 +2055,10 @@
         <v>47</v>
       </c>
       <c r="C42">
-        <v>215</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2083,7 +2070,7 @@
         <v>131</v>
       </c>
       <c r="H42" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2094,10 +2081,10 @@
         <v>48</v>
       </c>
       <c r="C43">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2109,7 +2096,7 @@
         <v>132</v>
       </c>
       <c r="H43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2120,10 +2107,10 @@
         <v>49</v>
       </c>
       <c r="C44">
-        <v>423</v>
+        <v>329</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2135,7 +2122,7 @@
         <v>133</v>
       </c>
       <c r="H44" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2146,10 +2133,10 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2161,7 +2148,7 @@
         <v>134</v>
       </c>
       <c r="H45" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2172,10 +2159,10 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2184,10 +2171,10 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="H46" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2198,10 +2185,10 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>4117</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2210,10 +2197,10 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2224,10 +2211,10 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>999</v>
+        <v>3141</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2236,10 +2223,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2250,10 +2237,10 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2262,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2276,22 +2263,22 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="D50" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="H50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2302,10 +2289,10 @@
         <v>56</v>
       </c>
       <c r="C51">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2314,16 +2301,13 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" location="Tesla%20#TSLA%20#TeslaStock%20#ElonMusk%20#SenatorKaren%20https://t.co/2Ah7lBRlXl"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>